<commit_message>
12te kjøp av vin
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Top 5" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -609,7 +609,7 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -680,6 +680,16 @@
     <xf numFmtId="166" fontId="7" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -698,16 +708,8 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -718,6 +720,12 @@
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -733,18 +741,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="0.0\ %"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -818,6 +814,12 @@
         <i val="0"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0\ %"/>
     </dxf>
     <dxf>
       <font>
@@ -1026,19 +1028,19 @@
     <tableColumn id="5" name="(pr - μ)/σ" dataDxfId="21">
       <calculatedColumnFormula>(F2-H2)/I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="prob" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="15" name="prob" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F2&gt;H2,1-_xlfn.NORM.DIST(F2,H2,I2,1),_xlfn.NORM.DIST(F2,H2,I2,1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="rank" dataDxfId="20">
+    <tableColumn id="6" name="rank" dataDxfId="19">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="cost" dataDxfId="19">
+    <tableColumn id="8" name="cost" dataDxfId="18">
       <calculatedColumnFormula>SUMIF(Sales!B:B,A2,Sales!E:E)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="cost/μ" dataDxfId="18">
+    <tableColumn id="4" name="cost/μ" dataDxfId="17">
       <calculatedColumnFormula>M2/H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="#i" dataDxfId="17">
+    <tableColumn id="14" name="#i" dataDxfId="16">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N2)+1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1058,15 +1060,15 @@
   </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="id" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="date" dataDxfId="16"/>
-    <tableColumn id="4" name="cost" dataDxfId="15"/>
-    <tableColumn id="3" name="sales" dataDxfId="14">
+    <tableColumn id="2" name="date" dataDxfId="15"/>
+    <tableColumn id="4" name="cost" dataDxfId="14"/>
+    <tableColumn id="3" name="sales" dataDxfId="13">
       <calculatedColumnFormula>SUMIFS(Sales!D:D,Sales!C:C,A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="prizes" totalsRowFunction="sum" dataDxfId="13">
+    <tableColumn id="5" name="prizes" totalsRowFunction="sum" dataDxfId="12">
       <calculatedColumnFormula>SUMIFS(Prizes!D:D,Prizes!C:C,A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="µ/ticket" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="6" name="µ/ticket" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>E2/D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1088,15 +1090,15 @@
   <tableColumns count="7">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="person_id"/>
-    <tableColumn id="3" name="lottery_id" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="lottery_id" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="4" name="tickets"/>
-    <tableColumn id="5" name="cost" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="5" name="cost" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>INDEX(Lotteries!C:C,MATCH(C2,Lotteries!A:A,0))*D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="µ" dataDxfId="6">
+    <tableColumn id="6" name="µ" dataDxfId="5">
       <calculatedColumnFormula>D2*INDEX(Lotteries!F:F,MATCH(C2,Lotteries!A:A,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="σ2" dataDxfId="5">
+    <tableColumn id="7" name="σ2" dataDxfId="4">
       <calculatedColumnFormula>INDEX(Lotteries!E:E,MATCH(C2,Lotteries!A:A,0))*D2/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-D2)/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-INDEX(Lotteries!E:E,MATCH(C2,Lotteries!A:A,0)))/(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1105,7 +1107,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Prizes" displayName="Prizes" ref="A1:D85" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Prizes" displayName="Prizes" ref="A1:D85" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D85">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1125,8 +1127,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:D13">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1134,8 +1136,8 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="date" dataDxfId="4"/>
-    <tableColumn id="4" name="cost" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="date" dataDxfId="1"/>
+    <tableColumn id="4" name="cost" dataDxfId="0" dataCellStyle="Comma"/>
     <tableColumn id="3" name="prizes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -1407,7 +1409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -1420,30 +1422,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="59" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
@@ -1918,30 +1920,30 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="60" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="16" t="s">
@@ -2416,30 +2418,30 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="61" t="s">
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="71"/>
+      <c r="R18" s="71"/>
+      <c r="S18" s="71"/>
+      <c r="T18" s="71"/>
+      <c r="U18" s="71"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
@@ -3004,49 +3006,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="65" t="s">
+      <c r="B1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="M1" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="64" t="s">
+      <c r="N1" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="O1" s="57" t="s">
         <v>94</v>
       </c>
       <c r="P1" s="29"/>
@@ -3073,7 +3075,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="35" t="str">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D2)+1)</f>
+        <f t="shared" ref="E2:E46" si="0">IF($C2=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F2" s="35">
@@ -3081,7 +3083,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="35" t="str">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F2)+1)</f>
+        <f t="shared" ref="G2:G46" si="1">IF($C2=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H2" s="36">
@@ -3093,15 +3095,15 @@
         <v>0.90534417201851047</v>
       </c>
       <c r="J2" s="36">
-        <f>(F2-H2)/I2</f>
+        <f t="shared" ref="J2:J46" si="2">(F2-H2)/I2</f>
         <v>-1.0911366986652986</v>
       </c>
       <c r="K2" s="49">
-        <f t="shared" ref="K2:K46" si="0">IF(F2&gt;H2,1-_xlfn.NORM.DIST(F2,H2,I2,1),_xlfn.NORM.DIST(F2,H2,I2,1))</f>
+        <f t="shared" ref="K2:K46" si="3">IF(F2&gt;H2,1-_xlfn.NORM.DIST(F2,H2,I2,1),_xlfn.NORM.DIST(F2,H2,I2,1))</f>
         <v>0.137606368366785</v>
       </c>
       <c r="L2" s="37" t="str">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</f>
+        <f t="shared" ref="L2:L46" si="4">IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M2" s="35">
@@ -3109,11 +3111,11 @@
         <v>100</v>
       </c>
       <c r="N2" s="31">
-        <f>M2/H2</f>
+        <f t="shared" ref="N2:N46" si="5">M2/H2</f>
         <v>101.22950819672131</v>
       </c>
       <c r="O2" s="31" t="str">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N2)+1)</f>
+        <f t="shared" ref="O2:O46" si="6">IF($C2=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3132,7 +3134,7 @@
         <v>102</v>
       </c>
       <c r="E3" s="29">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D3)+1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F3" s="29">
@@ -3140,7 +3142,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="29">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F3)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H3" s="30">
@@ -3152,15 +3154,15 @@
         <v>2.0742542497121694</v>
       </c>
       <c r="J3" s="30">
-        <f>(F3-H3)/I3</f>
+        <f t="shared" si="2"/>
         <v>-0.97570370398080453</v>
       </c>
       <c r="K3" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.16460565809130867</v>
       </c>
       <c r="L3" s="29">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J3)+1)</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="M3" s="29">
@@ -3168,11 +3170,11 @@
         <v>1110</v>
       </c>
       <c r="N3" s="31">
-        <f>M3/H3</f>
+        <f t="shared" si="5"/>
         <v>220.94575492462749</v>
       </c>
       <c r="O3" s="29">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N3)+1)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="P3" s="29"/>
@@ -3192,7 +3194,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="29">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D4)+1)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F4" s="29">
@@ -3200,7 +3202,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="29">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F4)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H4" s="30">
@@ -3212,15 +3214,15 @@
         <v>1.4405480167928464</v>
       </c>
       <c r="J4" s="30">
-        <f>(F4-H4)/I4</f>
+        <f t="shared" si="2"/>
         <v>-0.2247272290975878</v>
       </c>
       <c r="K4" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.41109574029874496</v>
       </c>
       <c r="L4" s="29">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J4)+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="M4" s="29">
@@ -3228,11 +3230,11 @@
         <v>550</v>
       </c>
       <c r="N4" s="31">
-        <f>M4/H4</f>
+        <f t="shared" si="5"/>
         <v>236.6883905613229</v>
       </c>
       <c r="O4" s="29">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N4)+1)</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="P4" s="29"/>
@@ -3252,7 +3254,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="29">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D5)+1)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F5" s="29">
@@ -3260,7 +3262,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="29">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F5)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H5" s="30">
@@ -3272,15 +3274,15 @@
         <v>1.2196223879112047</v>
       </c>
       <c r="J5" s="30">
-        <f>(F5-H5)/I5</f>
+        <f t="shared" si="2"/>
         <v>0.21426238923465521</v>
       </c>
       <c r="K5" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.41517122299034059</v>
       </c>
       <c r="L5" s="29">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J5)+1)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="M5" s="29">
@@ -3288,11 +3290,11 @@
         <v>350</v>
       </c>
       <c r="N5" s="31">
-        <f>M5/H5</f>
+        <f t="shared" si="5"/>
         <v>201.3020454176737</v>
       </c>
       <c r="O5" s="29">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N5)+1)</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P5" s="29"/>
@@ -3312,7 +3314,7 @@
         <v>55</v>
       </c>
       <c r="E6" s="29" t="str">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D6)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F6" s="29">
@@ -3320,7 +3322,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="29" t="str">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F6)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="30">
@@ -3332,15 +3334,15 @@
         <v>1.4608189121183603</v>
       </c>
       <c r="J6" s="30">
-        <f>(F6-H6)/I6</f>
+        <f t="shared" si="2"/>
         <v>0.42847177024759042</v>
       </c>
       <c r="K6" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.33415384099578926</v>
       </c>
       <c r="L6" s="29" t="str">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J6)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M6" s="29">
@@ -3348,11 +3350,11 @@
         <v>580</v>
       </c>
       <c r="N6" s="31">
-        <f>M6/H6</f>
+        <f t="shared" si="5"/>
         <v>244.30512797706007</v>
       </c>
       <c r="O6" s="29" t="str">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N6)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P6" s="29"/>
@@ -3372,7 +3374,7 @@
         <v>64</v>
       </c>
       <c r="E7" s="29">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D7)+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F7" s="29">
@@ -3380,7 +3382,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="29">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F7)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H7" s="30">
@@ -3392,15 +3394,15 @@
         <v>1.6246358262190024</v>
       </c>
       <c r="J7" s="30">
-        <f>(F7-H7)/I7</f>
+        <f t="shared" si="2"/>
         <v>0.64486200260527571</v>
       </c>
       <c r="K7" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.259508308715931</v>
       </c>
       <c r="L7" s="29">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J7)+1)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="M7" s="29">
@@ -3408,11 +3410,11 @@
         <v>740</v>
       </c>
       <c r="N7" s="31">
-        <f>M7/H7</f>
+        <f t="shared" si="5"/>
         <v>250.64913998317971</v>
       </c>
       <c r="O7" s="29">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N7)+1)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="P7" s="29"/>
@@ -3432,7 +3434,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="29" t="str">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D8)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F8" s="29">
@@ -3440,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="29" t="str">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F8)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H8" s="30">
@@ -3452,15 +3454,15 @@
         <v>1.1960152226849081</v>
       </c>
       <c r="J8" s="30">
-        <f>(F8-H8)/I8</f>
+        <f t="shared" si="2"/>
         <v>0.29081541460884686</v>
       </c>
       <c r="K8" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.38559624774223478</v>
       </c>
       <c r="L8" s="29" t="str">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J8)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M8" s="29">
@@ -3468,11 +3470,11 @@
         <v>350</v>
       </c>
       <c r="N8" s="31">
-        <f>M8/H8</f>
+        <f t="shared" si="5"/>
         <v>211.8412815677431</v>
       </c>
       <c r="O8" s="31" t="str">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N8)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P8" s="29"/>
@@ -3492,7 +3494,7 @@
         <v>75</v>
       </c>
       <c r="E9" s="29">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D9)+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F9" s="29">
@@ -3500,7 +3502,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="29">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F9)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H9" s="30">
@@ -3512,15 +3514,15 @@
         <v>1.645289709282524</v>
       </c>
       <c r="J9" s="30">
-        <f>(F9-H9)/I9</f>
+        <f t="shared" si="2"/>
         <v>0.55412515952783847</v>
       </c>
       <c r="K9" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.28974659632997213</v>
       </c>
       <c r="L9" s="29">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J9)+1)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="M9" s="29">
@@ -3528,11 +3530,11 @@
         <v>800</v>
       </c>
       <c r="N9" s="31">
-        <f>M9/H9</f>
+        <f t="shared" si="5"/>
         <v>259.04189143224175</v>
       </c>
       <c r="O9" s="29">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N9)+1)</f>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="P9" s="29"/>
@@ -3552,7 +3554,7 @@
         <v>157</v>
       </c>
       <c r="E10" s="29">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D10)+1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F10" s="29">
@@ -3560,7 +3562,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="29">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F10)+1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H10" s="30">
@@ -3572,15 +3574,15 @@
         <v>2.4711886604511184</v>
       </c>
       <c r="J10" s="30">
-        <f>(F10-H10)/I10</f>
+        <f t="shared" si="2"/>
         <v>0.30226024766922233</v>
       </c>
       <c r="K10" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.38122683981814831</v>
       </c>
       <c r="L10" s="29">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J10)+1)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="M10" s="29">
@@ -3588,11 +3590,11 @@
         <v>1740</v>
       </c>
       <c r="N10" s="31">
-        <f>M10/H10</f>
+        <f t="shared" si="5"/>
         <v>239.89881552872043</v>
       </c>
       <c r="O10" s="29">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N10)+1)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="P10" s="29"/>
@@ -3612,7 +3614,7 @@
         <v>68</v>
       </c>
       <c r="E11" s="29" t="str">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D11)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F11" s="29">
@@ -3620,7 +3622,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="29" t="str">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F11)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H11" s="30">
@@ -3632,15 +3634,15 @@
         <v>1.6903967309717229</v>
       </c>
       <c r="J11" s="30">
-        <f>(F11-H11)/I11</f>
+        <f t="shared" si="2"/>
         <v>2.224200373221318</v>
       </c>
       <c r="K11" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.3067482981361178E-2</v>
       </c>
       <c r="L11" s="29" t="str">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J11)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M11" s="29">
@@ -3648,11 +3650,11 @@
         <v>720</v>
       </c>
       <c r="N11" s="31">
-        <f>M11/H11</f>
+        <f t="shared" si="5"/>
         <v>222.20720539888777</v>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N11)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P11" s="29"/>
@@ -3672,7 +3674,7 @@
         <v>120</v>
       </c>
       <c r="E12" s="29">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D12)+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F12" s="29">
@@ -3680,7 +3682,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="29">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F12)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H12" s="30">
@@ -3692,15 +3694,15 @@
         <v>2.1775157131870162</v>
       </c>
       <c r="J12" s="30">
-        <f>(F12-H12)/I12</f>
+        <f t="shared" si="2"/>
         <v>-1.0901818568680326</v>
       </c>
       <c r="K12" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.13781652188722632</v>
       </c>
       <c r="L12" s="29">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J12)+1)</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="M12" s="29">
@@ -3708,11 +3710,11 @@
         <v>1300</v>
       </c>
       <c r="N12" s="31">
-        <f>M12/H12</f>
+        <f t="shared" si="5"/>
         <v>241.91050690099334</v>
       </c>
       <c r="O12" s="29">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N12)+1)</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="P12" s="29"/>
@@ -3732,7 +3734,7 @@
         <v>39</v>
       </c>
       <c r="E13" s="29">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D13)+1)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F13" s="29">
@@ -3740,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="29">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F13)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H13" s="30">
@@ -3752,15 +3754,15 @@
         <v>1.3415151969039836</v>
       </c>
       <c r="J13" s="30">
-        <f>(F13-H13)/I13</f>
+        <f t="shared" si="2"/>
         <v>-1.5116432729091189</v>
       </c>
       <c r="K13" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.5312318472907513E-2</v>
       </c>
       <c r="L13" s="29">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J13)+1)</f>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="M13" s="29">
@@ -3768,11 +3770,11 @@
         <v>460</v>
       </c>
       <c r="N13" s="31">
-        <f>M13/H13</f>
+        <f t="shared" si="5"/>
         <v>226.83649034053852</v>
       </c>
       <c r="O13" s="29">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N13)+1)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="P13" s="29"/>
@@ -3792,7 +3794,7 @@
         <v>48</v>
       </c>
       <c r="E14" s="29" t="str">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D14)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F14" s="29">
@@ -3800,7 +3802,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="29" t="str">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F14)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H14" s="30">
@@ -3812,15 +3814,15 @@
         <v>1.3966272062273601</v>
       </c>
       <c r="J14" s="30">
-        <f>(F14-H14)/I14</f>
+        <f t="shared" si="2"/>
         <v>0.59821503232865181</v>
       </c>
       <c r="K14" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27484823119819857</v>
       </c>
       <c r="L14" s="29" t="str">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J14)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M14" s="29">
@@ -3828,11 +3830,11 @@
         <v>530</v>
       </c>
       <c r="N14" s="31">
-        <f>M14/H14</f>
+        <f t="shared" si="5"/>
         <v>244.85836578291148</v>
       </c>
       <c r="O14" s="29" t="str">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N14)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P14" s="29"/>
@@ -3852,7 +3854,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="29">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D15)+1)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F15" s="29">
@@ -3860,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="29">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F15)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H15" s="30">
@@ -3872,15 +3874,15 @@
         <v>1.3555226273956775</v>
       </c>
       <c r="J15" s="30">
-        <f>(F15-H15)/I15</f>
+        <f t="shared" si="2"/>
         <v>-0.83309856993406151</v>
       </c>
       <c r="K15" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.20239457002747768</v>
       </c>
       <c r="L15" s="29">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J15)+1)</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="M15" s="29">
@@ -3888,11 +3890,11 @@
         <v>420</v>
       </c>
       <c r="N15" s="31">
-        <f>M15/H15</f>
+        <f t="shared" si="5"/>
         <v>197.2494075084621</v>
       </c>
       <c r="O15" s="29">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N15)+1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="P15" s="29"/>
@@ -3912,7 +3914,7 @@
         <v>73</v>
       </c>
       <c r="E16" s="29">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D16)+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F16" s="29">
@@ -3920,7 +3922,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="29">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F16)+1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H16" s="30">
@@ -3932,15 +3934,15 @@
         <v>1.7530186833491146</v>
       </c>
       <c r="J16" s="30">
-        <f>(F16-H16)/I16</f>
+        <f t="shared" si="2"/>
         <v>0.8647466592551053</v>
       </c>
       <c r="K16" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.19358892686978058</v>
       </c>
       <c r="L16" s="29">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J16)+1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M16" s="29">
@@ -3948,11 +3950,11 @@
         <v>770</v>
       </c>
       <c r="N16" s="31">
-        <f>M16/H16</f>
+        <f t="shared" si="5"/>
         <v>221.0050710785697</v>
       </c>
       <c r="O16" s="29">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N16)+1)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="P16" s="29"/>
@@ -3972,7 +3974,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="29">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D17)+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F17" s="29">
@@ -3980,7 +3982,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="29">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F17)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H17" s="30">
@@ -3992,15 +3994,15 @@
         <v>1.7690626415061241</v>
       </c>
       <c r="J17" s="30">
-        <f>(F17-H17)/I17</f>
+        <f t="shared" si="2"/>
         <v>0.24142041734861824</v>
       </c>
       <c r="K17" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.40461464495785371</v>
       </c>
       <c r="L17" s="29">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J17)+1)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="M17" s="29">
@@ -4008,11 +4010,11 @@
         <v>740</v>
       </c>
       <c r="N17" s="31">
-        <f>M17/H17</f>
+        <f t="shared" si="5"/>
         <v>207.11396393646277</v>
       </c>
       <c r="O17" s="29">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N17)+1)</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="P17" s="29"/>
@@ -4032,7 +4034,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="29">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D18)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F18" s="29">
@@ -4040,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="29">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F18)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H18" s="30">
@@ -4052,15 +4054,15 @@
         <v>0.70518688116242267</v>
       </c>
       <c r="J18" s="30">
-        <f>(F18-H18)/I18</f>
+        <f t="shared" si="2"/>
         <v>-0.76198633532411619</v>
       </c>
       <c r="K18" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.22303407988473595</v>
       </c>
       <c r="L18" s="29">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J18)+1)</f>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="M18" s="29">
@@ -4068,11 +4070,11 @@
         <v>140</v>
       </c>
       <c r="N18" s="31">
-        <f>M18/H18</f>
+        <f t="shared" si="5"/>
         <v>260.54133138258959</v>
       </c>
       <c r="O18" s="29">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N18)+1)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="P18" s="29"/>
@@ -4092,7 +4094,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="29">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D19)+1)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F19" s="29">
@@ -4100,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="29">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F19)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H19" s="30">
@@ -4112,15 +4114,15 @@
         <v>0.53561854612135185</v>
       </c>
       <c r="J19" s="30">
-        <f>(F19-H19)/I19</f>
+        <f t="shared" si="2"/>
         <v>-0.57282964535113001</v>
       </c>
       <c r="K19" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.28338002224276981</v>
       </c>
       <c r="L19" s="29">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J19)+1)</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="M19" s="29">
@@ -4128,11 +4130,11 @@
         <v>90</v>
       </c>
       <c r="N19" s="31">
-        <f>M19/H19</f>
+        <f t="shared" si="5"/>
         <v>293.33333333333331</v>
       </c>
       <c r="O19" s="29">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N19)+1)</f>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="P19" s="29"/>
@@ -4152,7 +4154,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="29">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D20)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F20" s="29">
@@ -4160,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="29">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F20)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H20" s="30">
@@ -4172,15 +4174,15 @@
         <v>0.78059289122728581</v>
       </c>
       <c r="J20" s="30">
-        <f>(F20-H20)/I20</f>
+        <f t="shared" si="2"/>
         <v>0.38068025533573507</v>
       </c>
       <c r="K20" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.35172026081826924</v>
       </c>
       <c r="L20" s="29">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J20)+1)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="M20" s="29">
@@ -4188,11 +4190,11 @@
         <v>150</v>
       </c>
       <c r="N20" s="31">
-        <f>M20/H20</f>
+        <f t="shared" si="5"/>
         <v>213.41871634405473</v>
       </c>
       <c r="O20" s="29">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N20)+1)</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="P20" s="29"/>
@@ -4212,7 +4214,7 @@
         <v>147</v>
       </c>
       <c r="E21" s="29" t="str">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D21)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F21" s="29">
@@ -4220,7 +4222,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="29" t="str">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F21)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H21" s="30">
@@ -4232,15 +4234,15 @@
         <v>2.1480307909963821</v>
       </c>
       <c r="J21" s="30">
-        <f>(F21-H21)/I21</f>
+        <f t="shared" si="2"/>
         <v>-0.6458180421064228</v>
       </c>
       <c r="K21" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.25919860106105741</v>
       </c>
       <c r="L21" s="29" t="str">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J21)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M21" s="29">
@@ -4248,11 +4250,11 @@
         <v>1570</v>
       </c>
       <c r="N21" s="31">
-        <f>M21/H21</f>
+        <f t="shared" si="5"/>
         <v>291.4295377006145</v>
       </c>
       <c r="O21" s="31" t="str">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N21)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P21" s="29"/>
@@ -4272,7 +4274,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="29">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D22)+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F22" s="29">
@@ -4280,7 +4282,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="29">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F22)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H22" s="30">
@@ -4292,15 +4294,15 @@
         <v>1.5154338440236188</v>
       </c>
       <c r="J22" s="30">
-        <f>(F22-H22)/I22</f>
+        <f t="shared" si="2"/>
         <v>0.32102335387251679</v>
       </c>
       <c r="K22" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.37409634649123846</v>
       </c>
       <c r="L22" s="29">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J22)+1)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="M22" s="29">
@@ -4308,11 +4310,11 @@
         <v>560</v>
       </c>
       <c r="N22" s="31">
-        <f>M22/H22</f>
+        <f t="shared" si="5"/>
         <v>222.79597979541578</v>
       </c>
       <c r="O22" s="29">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N22)+1)</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="P22" s="29"/>
@@ -4332,7 +4334,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="29" t="str">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D23)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F23" s="29">
@@ -4340,7 +4342,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="29" t="str">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F23)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H23" s="30">
@@ -4352,15 +4354,15 @@
         <v>0.75810728959235163</v>
       </c>
       <c r="J23" s="30">
-        <f>(F23-H23)/I23</f>
+        <f t="shared" si="2"/>
         <v>0.4858824982778579</v>
       </c>
       <c r="K23" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.31352523895390516</v>
       </c>
       <c r="L23" s="29" t="str">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J23)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M23" s="29">
@@ -4368,11 +4370,11 @@
         <v>200</v>
       </c>
       <c r="N23" s="31">
-        <f>M23/H23</f>
+        <f t="shared" si="5"/>
         <v>316.6315789473685</v>
       </c>
       <c r="O23" s="29" t="str">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N23)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P23" s="29"/>
@@ -4392,7 +4394,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="29">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D24)+1)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="F24" s="29">
@@ -4400,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="29">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F24)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H24" s="30">
@@ -4412,15 +4414,15 @@
         <v>0.67686632105875888</v>
       </c>
       <c r="J24" s="30">
-        <f>(F24-H24)/I24</f>
+        <f t="shared" si="2"/>
         <v>0.67477248464120332</v>
       </c>
       <c r="K24" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.24991016218462114</v>
       </c>
       <c r="L24" s="29">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J24)+1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M24" s="29">
@@ -4428,11 +4430,11 @@
         <v>100</v>
       </c>
       <c r="N24" s="31">
-        <f>M24/H24</f>
+        <f t="shared" si="5"/>
         <v>184.07079646017698</v>
       </c>
       <c r="O24" s="29">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N24)+1)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="P24" s="29"/>
@@ -4452,7 +4454,7 @@
         <v>75</v>
       </c>
       <c r="E25" s="29" t="str">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D25)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F25" s="29">
@@ -4460,7 +4462,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="29" t="str">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F25)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H25" s="30">
@@ -4472,15 +4474,15 @@
         <v>1.640793642686911</v>
       </c>
       <c r="J25" s="30">
-        <f>(F25-H25)/I25</f>
+        <f t="shared" si="2"/>
         <v>0.61000837120979057</v>
       </c>
       <c r="K25" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27092813112251135</v>
       </c>
       <c r="L25" s="29" t="str">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J25)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M25" s="29">
@@ -4488,11 +4490,11 @@
         <v>800</v>
       </c>
       <c r="N25" s="31">
-        <f>M25/H25</f>
+        <f t="shared" si="5"/>
         <v>266.74650011229147</v>
       </c>
       <c r="O25" s="29" t="str">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N25)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P25" s="29"/>
@@ -4512,7 +4514,7 @@
         <v>66</v>
       </c>
       <c r="E26" s="29">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D26)+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F26" s="29">
@@ -4520,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="29">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F26)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H26" s="30">
@@ -4532,15 +4534,15 @@
         <v>1.5620418614013669</v>
       </c>
       <c r="J26" s="30">
-        <f>(F26-H26)/I26</f>
+        <f t="shared" si="2"/>
         <v>-1.1068535147709484</v>
       </c>
       <c r="K26" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.13417863330317295</v>
       </c>
       <c r="L26" s="29">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J26)+1)</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="M26" s="29">
@@ -4548,11 +4550,11 @@
         <v>700</v>
       </c>
       <c r="N26" s="31">
-        <f>M26/H26</f>
+        <f t="shared" si="5"/>
         <v>256.50877038767311</v>
       </c>
       <c r="O26" s="29">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N26)+1)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="P26" s="29"/>
@@ -4572,7 +4574,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="29">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D27)+1)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F27" s="29">
@@ -4580,7 +4582,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="29">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F27)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H27" s="30">
@@ -4592,15 +4594,15 @@
         <v>0.24791576048881739</v>
       </c>
       <c r="J27" s="30">
-        <f>(F27-H27)/I27</f>
+        <f t="shared" si="2"/>
         <v>-0.25746562908380199</v>
       </c>
       <c r="K27" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.39840967257938792</v>
       </c>
       <c r="L27" s="29">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J27)+1)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="M27" s="29">
@@ -4608,11 +4610,11 @@
         <v>20</v>
       </c>
       <c r="N27" s="31">
-        <f>M27/H27</f>
+        <f t="shared" si="5"/>
         <v>313.33333333333337</v>
       </c>
       <c r="O27" s="29">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N27)+1)</f>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="P27" s="29"/>
@@ -4632,7 +4634,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="29" t="str">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D28)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F28" s="29">
@@ -4640,7 +4642,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="29" t="str">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F28)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H28" s="30">
@@ -4652,15 +4654,15 @@
         <v>0.54230382522055953</v>
       </c>
       <c r="J28" s="30">
-        <f>(F28-H28)/I28</f>
+        <f t="shared" si="2"/>
         <v>-0.58850578094375816</v>
       </c>
       <c r="K28" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27809642736849838</v>
       </c>
       <c r="L28" s="29" t="str">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J28)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M28" s="29">
@@ -4668,11 +4670,11 @@
         <v>100</v>
       </c>
       <c r="N28" s="31">
-        <f>M28/H28</f>
+        <f t="shared" si="5"/>
         <v>313.33333333333337</v>
       </c>
       <c r="O28" s="31" t="str">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N28)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P28" s="29"/>
@@ -4692,7 +4694,7 @@
         <v>11</v>
       </c>
       <c r="E29" s="29">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D29)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F29" s="29">
@@ -4700,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="29">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F29)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H29" s="30">
@@ -4712,15 +4714,15 @@
         <v>0.71401106976234563</v>
       </c>
       <c r="J29" s="30">
-        <f>(F29-H29)/I29</f>
+        <f t="shared" si="2"/>
         <v>-0.82094159664369926</v>
       </c>
       <c r="K29" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.20583976793322406</v>
       </c>
       <c r="L29" s="29">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J29)+1)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="M29" s="29">
@@ -4728,11 +4730,11 @@
         <v>100</v>
       </c>
       <c r="N29" s="31">
-        <f>M29/H29</f>
+        <f t="shared" si="5"/>
         <v>170.6014795754262</v>
       </c>
       <c r="O29" s="29">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N29)+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="P29" s="29"/>
@@ -4752,7 +4754,7 @@
         <v>24</v>
       </c>
       <c r="E30" s="29" t="str">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D30)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F30" s="29">
@@ -4760,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="29" t="str">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F30)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H30" s="30">
@@ -4772,15 +4774,15 @@
         <v>0.86060092285446455</v>
       </c>
       <c r="J30" s="30">
-        <f>(F30-H30)/I30</f>
+        <f t="shared" si="2"/>
         <v>-0.92277706012539296</v>
       </c>
       <c r="K30" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.17806169891377793</v>
       </c>
       <c r="L30" s="29" t="str">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J30)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M30" s="29">
@@ -4788,11 +4790,11 @@
         <v>240</v>
       </c>
       <c r="N30" s="31">
-        <f>M30/H30</f>
+        <f t="shared" si="5"/>
         <v>302.21265389966049</v>
       </c>
       <c r="O30" s="31" t="str">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N30)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P30" s="29"/>
@@ -4812,7 +4814,7 @@
         <v>51</v>
       </c>
       <c r="E31" s="29">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D31)+1)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F31" s="29">
@@ -4820,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="29">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F31)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H31" s="30">
@@ -4832,15 +4834,15 @@
         <v>1.3767007404782396</v>
       </c>
       <c r="J31" s="30">
-        <f>(F31-H31)/I31</f>
+        <f t="shared" si="2"/>
         <v>-0.10114828068400734</v>
       </c>
       <c r="K31" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.45971637604945381</v>
       </c>
       <c r="L31" s="29">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J31)+1)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="M31" s="29">
@@ -4848,11 +4850,11 @@
         <v>500</v>
       </c>
       <c r="N31" s="31">
-        <f>M31/H31</f>
+        <f t="shared" si="5"/>
         <v>233.7266736600364</v>
       </c>
       <c r="O31" s="29">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N31)+1)</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="P31" s="29"/>
@@ -4872,7 +4874,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="29" t="str">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D32)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F32" s="29">
@@ -4880,7 +4882,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="29" t="str">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F32)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H32" s="30">
@@ -4892,15 +4894,15 @@
         <v>0.43925136315935126</v>
       </c>
       <c r="J32" s="30">
-        <f>(F32-H32)/I32</f>
+        <f t="shared" si="2"/>
         <v>-0.47429183107111794</v>
       </c>
       <c r="K32" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.31764590799841352</v>
       </c>
       <c r="L32" s="29" t="str">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J32)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M32" s="29">
@@ -4908,11 +4910,11 @@
         <v>50</v>
       </c>
       <c r="N32" s="31">
-        <f>M32/H32</f>
+        <f t="shared" si="5"/>
         <v>240.00000000000003</v>
       </c>
       <c r="O32" s="31" t="str">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N32)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P32" s="29"/>
@@ -4932,7 +4934,7 @@
         <v>16</v>
       </c>
       <c r="E33" s="29" t="str">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D33)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F33" s="29">
@@ -4940,7 +4942,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="29" t="str">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F33)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H33" s="30">
@@ -4952,15 +4954,15 @@
         <v>0.79496113990168826</v>
       </c>
       <c r="J33" s="30">
-        <f>(F33-H33)/I33</f>
+        <f t="shared" si="2"/>
         <v>0.39856301064268529</v>
       </c>
       <c r="K33" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.34510761059987882</v>
       </c>
       <c r="L33" s="29" t="str">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J33)+1)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M33" s="29">
@@ -4968,11 +4970,11 @@
         <v>160</v>
       </c>
       <c r="N33" s="31">
-        <f>M33/H33</f>
+        <f t="shared" si="5"/>
         <v>234.20647149460706</v>
       </c>
       <c r="O33" s="31" t="str">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N33)+1)</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P33" s="29"/>
@@ -4992,7 +4994,7 @@
         <v>41</v>
       </c>
       <c r="E34" s="29">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D34)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F34" s="29">
@@ -5000,7 +5002,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="29">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F34)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H34" s="30">
@@ -5012,15 +5014,15 @@
         <v>1.2450174883944376</v>
       </c>
       <c r="J34" s="30">
-        <f>(F34-H34)/I34</f>
+        <f t="shared" si="2"/>
         <v>0.19973703231952852</v>
       </c>
       <c r="K34" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.42084312485409769</v>
       </c>
       <c r="L34" s="29">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J34)+1)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="M34" s="29">
@@ -5028,11 +5030,11 @@
         <v>400</v>
       </c>
       <c r="N34" s="31">
-        <f>M34/H34</f>
+        <f t="shared" si="5"/>
         <v>228.39864151673595</v>
       </c>
       <c r="O34" s="29">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N34)+1)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="P34" s="29"/>
@@ -5052,7 +5054,7 @@
         <v>82</v>
       </c>
       <c r="E35" s="29">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D35)+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F35" s="29">
@@ -5060,7 +5062,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="29">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F35)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H35" s="30">
@@ -5072,15 +5074,15 @@
         <v>1.8257369483316859</v>
       </c>
       <c r="J35" s="30">
-        <f>(F35-H35)/I35</f>
+        <f t="shared" si="2"/>
         <v>-0.43660492998348149</v>
       </c>
       <c r="K35" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.33119894334721611</v>
       </c>
       <c r="L35" s="29">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J35)+1)</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="M35" s="29">
@@ -5088,11 +5090,11 @@
         <v>810</v>
       </c>
       <c r="N35" s="31">
-        <f>M35/H35</f>
+        <f t="shared" si="5"/>
         <v>213.31924534441649</v>
       </c>
       <c r="O35" s="29">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N35)+1)</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="P35" s="29"/>
@@ -5112,7 +5114,7 @@
         <v>41</v>
       </c>
       <c r="E36" s="29">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D36)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F36" s="29">
@@ -5120,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="29">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F36)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H36" s="30">
@@ -5132,15 +5134,15 @@
         <v>1.3441673982599343</v>
       </c>
       <c r="J36" s="30">
-        <f>(F36-H36)/I36</f>
+        <f t="shared" si="2"/>
         <v>-0.74080480953425287</v>
       </c>
       <c r="K36" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.22940589929755095</v>
       </c>
       <c r="L36" s="29">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J36)+1)</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="M36" s="29">
@@ -5148,11 +5150,11 @@
         <v>400</v>
       </c>
       <c r="N36" s="31">
-        <f>M36/H36</f>
+        <f t="shared" si="5"/>
         <v>200.42433103306936</v>
       </c>
       <c r="O36" s="29">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N36)+1)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="P36" s="29"/>
@@ -5172,7 +5174,7 @@
         <v>36</v>
       </c>
       <c r="E37" s="29">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D37)+1)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F37" s="29">
@@ -5180,7 +5182,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="29">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F37)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H37" s="30">
@@ -5192,15 +5194,15 @@
         <v>1.2852767126125033</v>
       </c>
       <c r="J37" s="30">
-        <f>(F37-H37)/I37</f>
+        <f t="shared" si="2"/>
         <v>0.1312620147123815</v>
       </c>
       <c r="K37" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.44778401980729587</v>
       </c>
       <c r="L37" s="29">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J37)+1)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="M37" s="29">
@@ -5208,11 +5210,11 @@
         <v>350</v>
       </c>
       <c r="N37" s="31">
-        <f>M37/H37</f>
+        <f t="shared" si="5"/>
         <v>191.12189757643927</v>
       </c>
       <c r="O37" s="29">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N37)+1)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P37" s="29"/>
@@ -5232,7 +5234,7 @@
         <v>41</v>
       </c>
       <c r="E38" s="29">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D38)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F38" s="29">
@@ -5240,7 +5242,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="29">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F38)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H38" s="30">
@@ -5252,15 +5254,15 @@
         <v>1.3441673982599343</v>
       </c>
       <c r="J38" s="30">
-        <f>(F38-H38)/I38</f>
+        <f t="shared" si="2"/>
         <v>3.1501482295870731E-3</v>
       </c>
       <c r="K38" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.49874327476019131</v>
       </c>
       <c r="L38" s="29">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J38)+1)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="M38" s="29">
@@ -5268,11 +5270,11 @@
         <v>400</v>
       </c>
       <c r="N38" s="31">
-        <f>M38/H38</f>
+        <f t="shared" si="5"/>
         <v>200.42433103306936</v>
       </c>
       <c r="O38" s="29">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N38)+1)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="P38" s="29"/>
@@ -5292,7 +5294,7 @@
         <v>91</v>
       </c>
       <c r="E39" s="29">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D39)+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F39" s="29">
@@ -5300,7 +5302,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="29">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F39)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H39" s="30">
@@ -5312,15 +5314,15 @@
         <v>1.9032990868959521</v>
       </c>
       <c r="J39" s="30">
-        <f>(F39-H39)/I39</f>
+        <f t="shared" si="2"/>
         <v>-0.609868477383676</v>
       </c>
       <c r="K39" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.27097446775170275</v>
       </c>
       <c r="L39" s="29">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J39)+1)</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="M39" s="29">
@@ -5328,11 +5330,11 @@
         <v>900</v>
       </c>
       <c r="N39" s="31">
-        <f>M39/H39</f>
+        <f t="shared" si="5"/>
         <v>216.30652627574281</v>
       </c>
       <c r="O39" s="29">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N39)+1)</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P39" s="29"/>
@@ -5352,7 +5354,7 @@
         <v>37</v>
       </c>
       <c r="E40" s="35">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D40)+1)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F40" s="35">
@@ -5360,7 +5362,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="35">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F40)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H40" s="36">
@@ -5372,15 +5374,15 @@
         <v>1.2439598119364987</v>
       </c>
       <c r="J40" s="36">
-        <f>(F40-H40)/I40</f>
+        <f t="shared" si="2"/>
         <v>1.7963311108174056</v>
       </c>
       <c r="K40" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.6220936405928716E-2</v>
       </c>
       <c r="L40" s="37">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J40)+1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M40" s="35">
@@ -5388,11 +5390,11 @@
         <v>360</v>
       </c>
       <c r="N40" s="31">
-        <f>M40/H40</f>
+        <f t="shared" si="5"/>
         <v>203.9155999000713</v>
       </c>
       <c r="O40" s="29">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N40)+1)</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="P40" s="29"/>
@@ -5412,7 +5414,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="35">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D41)+1)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="F41" s="35">
@@ -5420,7 +5422,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="35">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F41)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H41" s="36">
@@ -5432,15 +5434,15 @@
         <v>0.54598817687849921</v>
       </c>
       <c r="J41" s="36">
-        <f>(F41-H41)/I41</f>
+        <f t="shared" si="2"/>
         <v>-0.66156013751613985</v>
       </c>
       <c r="K41" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.25412658085528567</v>
       </c>
       <c r="L41" s="37">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J41)+1)</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="M41" s="35">
@@ -5448,11 +5450,11 @@
         <v>20</v>
       </c>
       <c r="N41" s="31">
-        <f>M41/H41</f>
+        <f t="shared" si="5"/>
         <v>55.370370370370374</v>
       </c>
       <c r="O41" s="29">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N41)+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="P41" s="29"/>
@@ -5472,7 +5474,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="35">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D42)+1)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="F42" s="35">
@@ -5480,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="35">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F42)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H42" s="36">
@@ -5492,15 +5494,15 @@
         <v>0.42132504423474315</v>
       </c>
       <c r="J42" s="36">
-        <f>(F42-H42)/I42</f>
+        <f t="shared" si="2"/>
         <v>-0.54772255750516619</v>
       </c>
       <c r="K42" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.2919412103851825</v>
       </c>
       <c r="L42" s="37">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J42)+1)</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="M42" s="35">
@@ -5508,11 +5510,11 @@
         <v>0</v>
       </c>
       <c r="N42" s="31">
-        <f>M42/H42</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O42" s="29">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N42)+1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P42" s="29"/>
@@ -5532,7 +5534,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="37">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D43)+1)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F43" s="35">
@@ -5540,7 +5542,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="37">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F43)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H43" s="36">
@@ -5552,15 +5554,15 @@
         <v>0.73982863701939761</v>
       </c>
       <c r="J43" s="36">
-        <f>(F43-H43)/I43</f>
+        <f t="shared" si="2"/>
         <v>1.8930256409135764</v>
       </c>
       <c r="K43" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.9177229841034769E-2</v>
       </c>
       <c r="L43" s="37">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J43)+1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M43" s="35">
@@ -5568,11 +5570,11 @@
         <v>150</v>
       </c>
       <c r="N43" s="31">
-        <f>M43/H43</f>
+        <f t="shared" si="5"/>
         <v>250.21459227467813</v>
       </c>
       <c r="O43" s="37">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N43)+1)</f>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="P43" s="29"/>
@@ -5592,7 +5594,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="35">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D44)+1)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F44" s="35">
@@ -5600,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="35">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F44)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H44" s="36">
@@ -5612,15 +5614,15 @@
         <v>0.37094647870344777</v>
       </c>
       <c r="J44" s="36">
-        <f>(F44-H44)/I44</f>
+        <f t="shared" si="2"/>
         <v>-0.39211733715048613</v>
       </c>
       <c r="K44" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.34748575901730239</v>
       </c>
       <c r="L44" s="37">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J44)+1)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="M44" s="35">
@@ -5628,11 +5630,11 @@
         <v>40</v>
       </c>
       <c r="N44" s="31">
-        <f>M44/H44</f>
+        <f t="shared" si="5"/>
         <v>275</v>
       </c>
       <c r="O44" s="29">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N44)+1)</f>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="P44" s="29"/>
@@ -5652,7 +5654,7 @@
         <v>10</v>
       </c>
       <c r="E45" s="35">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D45)+1)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F45" s="35">
@@ -5660,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="35">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F45)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H45" s="36">
@@ -5672,15 +5674,15 @@
         <v>0.67996690791586989</v>
       </c>
       <c r="J45" s="36">
-        <f>(F45-H45)/I45</f>
+        <f t="shared" si="2"/>
         <v>0.72370413314432125</v>
       </c>
       <c r="K45" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.23462369757905566</v>
       </c>
       <c r="L45" s="37">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J45)+1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="M45" s="35">
@@ -5688,11 +5690,11 @@
         <v>100</v>
       </c>
       <c r="N45" s="31">
-        <f>M45/H45</f>
+        <f t="shared" si="5"/>
         <v>196.88715953307394</v>
       </c>
       <c r="O45" s="29">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N45)+1)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="P45" s="29"/>
@@ -5712,7 +5714,7 @@
         <v>5</v>
       </c>
       <c r="E46" s="35">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D46)+1)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="F46" s="35">
@@ -5720,7 +5722,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="35">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F46)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H46" s="36">
@@ -5732,15 +5734,15 @@
         <v>0.53983489724168388</v>
       </c>
       <c r="J46" s="36">
-        <f>(F46-H46)/I46</f>
+        <f t="shared" si="2"/>
         <v>1.2483688011309693</v>
       </c>
       <c r="K46" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.10594801446913715</v>
       </c>
       <c r="L46" s="37">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J46)+1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M46" s="35">
@@ -5748,11 +5750,11 @@
         <v>50</v>
       </c>
       <c r="N46" s="31">
-        <f>M46/H46</f>
+        <f t="shared" si="5"/>
         <v>153.33333333333334</v>
       </c>
       <c r="O46" s="29">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,N:N,"&lt;"&amp;N46)+1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="P46" s="29"/>
@@ -5779,22 +5781,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="56" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6166,25 +6168,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="62" t="s">
         <v>32</v>
       </c>
       <c r="I1" t="s">
@@ -13308,10 +13310,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13319,21 +13321,28 @@
     <col min="5" max="5" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="60" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1">
+        <f>SUM(D:D)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13347,7 +13356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13361,7 +13370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13375,7 +13384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13389,7 +13398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13403,7 +13412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13417,7 +13426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13431,7 +13440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13445,7 +13454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13459,7 +13468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13473,7 +13482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13487,7 +13496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13501,7 +13510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13515,7 +13524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13529,7 +13538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -14523,29 +14532,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.08984375" style="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="60" t="s">
         <v>21</v>
       </c>
       <c r="F1" t="s">
@@ -14553,10 +14563,14 @@
       </c>
       <c r="G1" s="40">
         <f>SUM(C:C)</f>
-        <v>20124.150000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>23114.15</v>
+      </c>
+      <c r="H1" s="39">
+        <f>SUM(D:D)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -14570,7 +14584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -14584,7 +14598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -14598,7 +14612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -14612,7 +14626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -14626,7 +14640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -14640,7 +14654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -14654,7 +14668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -14668,7 +14682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -14682,7 +14696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -14696,7 +14710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -14707,6 +14721,20 @@
         <v>2894</v>
       </c>
       <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43704</v>
+      </c>
+      <c r="C13" s="41">
+        <v>2990</v>
+      </c>
+      <c r="D13">
         <v>12</v>
       </c>
     </row>
@@ -14720,26 +14748,33 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="39"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="40">
         <v>3929</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>98</v>
       </c>
@@ -14747,8 +14782,15 @@
         <f>Sales!J1</f>
         <v>20720</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="39">
+        <f>Purchases!H1</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>65</v>
       </c>
@@ -14757,22 +14799,36 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="42" t="s">
         <v>96</v>
       </c>
       <c r="C5" s="43">
         <f>-Purchases!G1</f>
-        <v>-20124.150000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+        <v>-23114.15</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="72">
+        <f>-Prizes!G1</f>
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="64">
         <f>SUM(C2:C5)</f>
-        <v>4424.8499999999985</v>
+        <v>1434.8499999999985</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="73">
+        <f>SUM(G1:G5)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OB for innkjøp, lagt til renter i database
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Top 5" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -397,6 +397,21 @@
   <si>
     <t>standard deviation of prizes</t>
   </si>
+  <si>
+    <t>Renter</t>
+  </si>
+  <si>
+    <t>Renter 2016</t>
+  </si>
+  <si>
+    <t>Renter 2017</t>
+  </si>
+  <si>
+    <t>Renter 2018</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
 </sst>
 </file>
 
@@ -486,6 +501,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -690,6 +706,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -708,8 +726,6 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1410,7 +1426,7 @@
   <dimension ref="B2:U41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,30 +1438,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
@@ -1920,30 +1936,30 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="70" t="s">
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="16" t="s">
@@ -2418,30 +2434,30 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="71" t="s">
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="71"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="71"/>
-      <c r="S18" s="71"/>
-      <c r="T18" s="71"/>
-      <c r="U18" s="71"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
@@ -2988,8 +3004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5772,7 +5788,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6157,8 +6173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J274"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E264" sqref="E264"/>
+    <sheetView topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14534,8 +14550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14748,33 +14764,34 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G6"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" customWidth="1"/>
     <col min="7" max="7" width="8.90625" style="39"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="40">
         <v>3929</v>
       </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>98</v>
       </c>
@@ -14782,53 +14799,84 @@
         <f>Sales!J1</f>
         <v>20720</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="40">
+        <f>J7</f>
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J4" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="40">
+        <f>-Persons!R1</f>
+        <v>-100</v>
+      </c>
+      <c r="F5" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G5" s="39">
         <f>Purchases!H1</f>
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="40">
-        <f>-Persons!R1</f>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="42" t="s">
+      <c r="J5" s="40"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C6" s="43">
         <f>-Purchases!G1</f>
         <v>-23114.15</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F6" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G6" s="66">
         <f>-Prizes!G1</f>
         <v>-90</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="63" t="s">
+      <c r="I6" s="42"/>
+      <c r="J6" s="43"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="64">
-        <f>SUM(C2:C5)</f>
-        <v>1434.8499999999985</v>
-      </c>
-      <c r="F6" s="63" t="s">
+      <c r="C7" s="64">
+        <f>SUM(C2:C6)</f>
+        <v>1460.8499999999985</v>
+      </c>
+      <c r="F7" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="73">
-        <f>SUM(G1:G5)</f>
+      <c r="G7" s="67">
+        <f>SUM(G2:G6)</f>
         <v>12</v>
+      </c>
+      <c r="I7" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="64">
+        <f>SUM(J2:J6)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rettelser til mai trekkning
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="9225" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="9225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Top 5" sheetId="7" r:id="rId1"/>
@@ -1136,25 +1136,6 @@
   </cellStyles>
   <dxfs count="41">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
@@ -1175,6 +1156,25 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1531,8 +1531,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Persons" displayName="Persons" ref="A1:U57" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:U57"/>
-  <sortState ref="A2:U51">
-    <sortCondition ref="A1:A51"/>
+  <sortState ref="A2:U57">
+    <sortCondition ref="A1:A57"/>
   </sortState>
   <tableColumns count="21">
     <tableColumn id="1" name="id" dataDxfId="38"/>
@@ -1639,15 +1639,15 @@
   <tableColumns count="7">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="person_id"/>
-    <tableColumn id="3" name="lottery_id" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="lottery_id" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="4" name="tickets"/>
-    <tableColumn id="5" name="cost" dataDxfId="2" totalsRowDxfId="3">
+    <tableColumn id="5" name="cost" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>INDEX(Lotteries!C:C,MATCH(C2,Lotteries!A:A,0))*D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="µ" dataDxfId="1">
+    <tableColumn id="6" name="µ" dataDxfId="5">
       <calculatedColumnFormula>D2*INDEX(Lotteries!G:G,MATCH(C2,Lotteries!A:A,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="σ2" dataDxfId="0">
+    <tableColumn id="7" name="σ2" dataDxfId="4">
       <calculatedColumnFormula>INDEX(Lotteries!F:F,MATCH(C2,Lotteries!A:A,0))*D2/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-D2)/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-INDEX(Lotteries!F:F,MATCH(C2,Lotteries!A:A,0)))/(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1656,7 +1656,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Prizes" displayName="Prizes" ref="A1:D118" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Prizes" displayName="Prizes" ref="A1:D118" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D118">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1674,7 +1674,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:E17">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1684,8 +1684,8 @@
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="date" dataDxfId="7"/>
-    <tableColumn id="4" name="cost" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="date" dataDxfId="1"/>
+    <tableColumn id="4" name="cost" dataDxfId="0" dataCellStyle="Comma"/>
     <tableColumn id="3" name="prizes"/>
     <tableColumn id="5" name="faktura"/>
   </tableColumns>
@@ -1961,8 +1961,8 @@
   </sheetPr>
   <dimension ref="B2:Z27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,15 +2153,15 @@
       </c>
       <c r="G6" s="38">
         <f t="array" ref="G6">INDEX(Persons!$A:$A,SMALL(IF(Persons!$Q:$Q=F6,ROW(Persons!$A:$A)-ROW(Persons!$A$1)+1),COUNTIF(F$4:F6,F6)))</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H6" s="38" t="str">
         <f>INDEX(Persons!$B:$B,MATCH(G6,Persons!$A:$A,0))</f>
-        <v>Fridtjof</v>
+        <v>Kenneth</v>
       </c>
       <c r="I6" s="70">
         <f>INDEX(Persons!$R:$R,MATCH(G6,Persons!$A:$A,0))</f>
-        <v>0.12701859000624371</v>
+        <v>9.4842360181836213E-2</v>
       </c>
       <c r="J6" s="39">
         <f>SMALL(Persons!$S:$S,1+ROW(J6)-ROW(J$4))</f>
@@ -2203,15 +2203,15 @@
       </c>
       <c r="G7" s="38">
         <f t="array" ref="G7">INDEX(Persons!$A:$A,SMALL(IF(Persons!$Q:$Q=F7,ROW(Persons!$A:$A)-ROW(Persons!$A$1)+1),COUNTIF(F$4:F7,F7)))</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H7" s="38" t="str">
         <f>INDEX(Persons!$B:$B,MATCH(G7,Persons!$A:$A,0))</f>
-        <v>Ruben O</v>
+        <v>Fridtjof</v>
       </c>
       <c r="I7" s="70">
         <f>INDEX(Persons!$R:$R,MATCH(G7,Persons!$A:$A,0))</f>
-        <v>0.12986049313998585</v>
+        <v>0.12701859000624371</v>
       </c>
       <c r="J7" s="39">
         <f>SMALL(Persons!$S:$S,1+ROW(J7)-ROW(J$4))</f>
@@ -2257,15 +2257,15 @@
       </c>
       <c r="G8" s="38">
         <f t="array" ref="G8">INDEX(Persons!$A:$A,SMALL(IF(Persons!$Q:$Q=F8,ROW(Persons!$A:$A)-ROW(Persons!$A$1)+1),COUNTIF(F$4:F8,F8)))</f>
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H8" s="38" t="str">
         <f>INDEX(Persons!$B:$B,MATCH(G8,Persons!$A:$A,0))</f>
-        <v>Kenneth</v>
+        <v>Ruben O</v>
       </c>
       <c r="I8" s="70">
         <f>INDEX(Persons!$R:$R,MATCH(G8,Persons!$A:$A,0))</f>
-        <v>0.1341301701833536</v>
+        <v>0.12986049313998585</v>
       </c>
       <c r="J8" s="39">
         <f>SMALL(Persons!$S:$S,1+ROW(J8)-ROW(J$4))</f>
@@ -2627,15 +2627,15 @@
       </c>
       <c r="K15" s="56">
         <f t="array" ref="K15">INDEX(Persons!$A:$A,SMALL(IF(Persons!$O:$O=J15,ROW(Persons!$A:$A)-ROW(Persons!$A$1)+1),COUNTIF(J$12:J15,J15)))</f>
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="L15" s="56" t="str">
         <f>INDEX(Persons!$B:$B,MATCH(K15,Persons!$A:$A,0))</f>
-        <v>Asgeir</v>
+        <v>Kenneth</v>
       </c>
       <c r="M15" s="73">
         <f>INDEX(Persons!$N:$N,MATCH(K15,Persons!$A:$A,0))</f>
-        <v>-1.3959495602492105</v>
+        <v>-1.5492461951326595</v>
       </c>
       <c r="U15">
         <v>7</v>
@@ -2691,15 +2691,15 @@
       </c>
       <c r="K16" s="56">
         <f t="array" ref="K16">INDEX(Persons!$A:$A,SMALL(IF(Persons!$O:$O=J16,ROW(Persons!$A:$A)-ROW(Persons!$A$1)+1),COUNTIF(J$12:J16,J16)))</f>
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="L16" s="56" t="str">
         <f>INDEX(Persons!$B:$B,MATCH(K16,Persons!$A:$A,0))</f>
-        <v>Fridtjof</v>
+        <v>Asgeir</v>
       </c>
       <c r="M16" s="73">
         <f>INDEX(Persons!$N:$N,MATCH(K16,Persons!$A:$A,0))</f>
-        <v>-1.184672257882758</v>
+        <v>-1.3959495602492105</v>
       </c>
       <c r="U16">
         <v>8</v>
@@ -3080,8 +3080,8 @@
   </sheetPr>
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3190,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="6" t="str">
-        <f t="shared" ref="F2:F33" si="0">IF($C2=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G2" s="8">
@@ -3198,7 +3198,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="8" t="str">
-        <f t="shared" ref="H2:H33" si="1">IF($C2=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I2" s="8">
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="8" t="str">
-        <f t="shared" ref="J2:J33" si="2">IF($C2=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K2" s="9">
@@ -3214,7 +3214,7 @@
         <v>0.98785425101214575</v>
       </c>
       <c r="L2" s="30" t="str">
-        <f t="shared" ref="L2:L33" si="3">IF($C2=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M2" s="9">
@@ -3222,35 +3222,35 @@
         <v>0.90534417201851047</v>
       </c>
       <c r="N2" s="9">
-        <f t="shared" ref="N2:N33" si="4">I2-K2</f>
+        <f>I2-K2</f>
         <v>-0.98785425101214575</v>
       </c>
       <c r="O2" s="6" t="str">
-        <f t="shared" ref="O2:O33" si="5">IF($C2=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P2" s="5">
-        <f t="shared" ref="P2:P33" si="6">N2/M2</f>
+        <f>N2/M2</f>
         <v>-1.0911366986652986</v>
       </c>
       <c r="Q2" s="10" t="str">
-        <f t="shared" ref="Q2:Q33" si="7">IF($C2=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R2" s="17">
-        <f t="shared" ref="R2:R33" si="8">IF(I2&gt;K2,1-_xlfn.NORM.DIST(I2,K2,M2,1),_xlfn.NORM.DIST(I2,K2,M2,1))</f>
+        <f>IF(I2&gt;K2,1-_xlfn.NORM.DIST(I2,K2,M2,1),_xlfn.NORM.DIST(I2,K2,M2,1))</f>
         <v>0.137606368366785</v>
       </c>
       <c r="S2" s="6" t="str">
-        <f t="shared" ref="S2:S33" si="9">IF($C2=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T2" s="6">
-        <f t="shared" ref="T2:T33" si="10">E2/K2</f>
+        <f>E2/K2</f>
         <v>101.22950819672131</v>
       </c>
       <c r="U2" s="6" t="str">
-        <f t="shared" ref="U2:U33" si="11">IF($C2=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T2)+1)</f>
+        <f>IF($C2=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T2)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="X2" s="4"/>
@@ -3275,7 +3275,7 @@
         <v>1360</v>
       </c>
       <c r="F3" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G3" s="4">
@@ -3283,7 +3283,7 @@
         <v>127</v>
       </c>
       <c r="H3" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I3" s="4">
@@ -3291,7 +3291,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K3" s="5">
@@ -3299,7 +3299,7 @@
         <v>6.0719704412152948</v>
       </c>
       <c r="L3" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M3" s="5">
@@ -3307,35 +3307,35 @@
         <v>2.2871608424340759</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" si="4"/>
+        <f>I3-K3</f>
         <v>-1.0719704412152948</v>
       </c>
       <c r="O3" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P3" s="5">
-        <f t="shared" si="6"/>
+        <f>N3/M3</f>
         <v>-0.46869044858011238</v>
       </c>
       <c r="Q3" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R3" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I3&gt;K3,1-_xlfn.NORM.DIST(I3,K3,M3,1),_xlfn.NORM.DIST(I3,K3,M3,1))</f>
         <v>0.3196454575746297</v>
       </c>
       <c r="S3" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T3" s="6">
-        <f t="shared" si="10"/>
+        <f>E3/K3</f>
         <v>223.98000997643169</v>
       </c>
       <c r="U3" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C3=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T3)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V3" s="4"/>
@@ -3361,7 +3361,7 @@
         <v>750</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E4)+1)</f>
         <v>10</v>
       </c>
       <c r="G4" s="4">
@@ -3369,7 +3369,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G4)+1)</f>
         <v>12</v>
       </c>
       <c r="I4" s="4">
@@ -3377,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I4)+1)</f>
         <v>11</v>
       </c>
       <c r="K4" s="5">
@@ -3385,7 +3385,7 @@
         <v>3.0749747879706155</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K4)+1)</f>
         <v>12</v>
       </c>
       <c r="M4" s="5">
@@ -3393,35 +3393,35 @@
         <v>1.6670556241583492</v>
       </c>
       <c r="N4" s="5">
-        <f t="shared" si="4"/>
+        <f>I4-K4</f>
         <v>-1.0749747879706155</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N4)+1)</f>
         <v>26</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" si="6"/>
+        <f>N4/M4</f>
         <v>-0.64483438488343237</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P4)+1)</f>
         <v>21</v>
       </c>
       <c r="R4" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I4&gt;K4,1-_xlfn.NORM.DIST(I4,K4,M4,1),_xlfn.NORM.DIST(I4,K4,M4,1))</f>
         <v>0.25951725827739575</v>
       </c>
       <c r="S4" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R4)+1)</f>
         <v>17</v>
       </c>
       <c r="T4" s="6">
-        <f t="shared" si="10"/>
+        <f>E4/K4</f>
         <v>243.90443880516364</v>
       </c>
       <c r="U4" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C4=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T4)+1)</f>
         <v>23</v>
       </c>
       <c r="V4" s="4"/>
@@ -3447,7 +3447,7 @@
         <v>350</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E5)+1)</f>
         <v>17</v>
       </c>
       <c r="G5" s="4">
@@ -3455,15 +3455,15 @@
         <v>26</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G5)+1)</f>
+        <v>22</v>
       </c>
       <c r="I5" s="4">
         <f>SUMIF(Prizes!B:B,A5,Prizes!D:D)</f>
         <v>2</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I5)+1)</f>
         <v>11</v>
       </c>
       <c r="K5" s="5">
@@ -3471,7 +3471,7 @@
         <v>1.7386807932020698</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K5)+1)</f>
         <v>17</v>
       </c>
       <c r="M5" s="5">
@@ -3479,35 +3479,35 @@
         <v>1.2196223879112047</v>
       </c>
       <c r="N5" s="5">
-        <f t="shared" si="4"/>
+        <f>I5-K5</f>
         <v>0.26131920679793019</v>
       </c>
       <c r="O5" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N5)+1)</f>
         <v>10</v>
       </c>
       <c r="P5" s="5">
-        <f t="shared" si="6"/>
+        <f>N5/M5</f>
         <v>0.21426238923465521</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P5)+1)</f>
         <v>11</v>
       </c>
       <c r="R5" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I5&gt;K5,1-_xlfn.NORM.DIST(I5,K5,M5,1),_xlfn.NORM.DIST(I5,K5,M5,1))</f>
         <v>0.41517122299034059</v>
       </c>
       <c r="S5" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R5)+1)</f>
         <v>4</v>
       </c>
       <c r="T5" s="6">
-        <f t="shared" si="10"/>
+        <f>E5/K5</f>
         <v>201.3020454176737</v>
       </c>
       <c r="U5" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C5=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T5)+1)</f>
         <v>2</v>
       </c>
       <c r="V5" s="4"/>
@@ -3533,7 +3533,7 @@
         <v>580</v>
       </c>
       <c r="F6" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G6" s="4">
@@ -3541,7 +3541,7 @@
         <v>55</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I6" s="4">
@@ -3549,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K6" s="5">
@@ -3557,7 +3557,7 @@
         <v>2.3740803347134869</v>
       </c>
       <c r="L6" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M6" s="5">
@@ -3565,35 +3565,35 @@
         <v>1.4608189121183603</v>
       </c>
       <c r="N6" s="5">
-        <f t="shared" si="4"/>
+        <f>I6-K6</f>
         <v>0.6259196652865131</v>
       </c>
       <c r="O6" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P6" s="5">
-        <f t="shared" si="6"/>
+        <f>N6/M6</f>
         <v>0.42847177024759042</v>
       </c>
       <c r="Q6" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R6" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I6&gt;K6,1-_xlfn.NORM.DIST(I6,K6,M6,1),_xlfn.NORM.DIST(I6,K6,M6,1))</f>
         <v>0.33415384099578926</v>
       </c>
       <c r="S6" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T6" s="6">
-        <f t="shared" si="10"/>
+        <f>E6/K6</f>
         <v>244.30512797706007</v>
       </c>
       <c r="U6" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C6=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T6)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V6" s="4"/>
@@ -3619,7 +3619,7 @@
         <v>790</v>
       </c>
       <c r="F7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G7" s="4">
@@ -3627,7 +3627,7 @@
         <v>69</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I7" s="4">
@@ -3635,7 +3635,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K7" s="5">
@@ -3643,7 +3643,7 @@
         <v>3.2250613603274099</v>
       </c>
       <c r="L7" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M7" s="5">
@@ -3651,35 +3651,35 @@
         <v>1.6993617556865768</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" si="4"/>
+        <f>I7-K7</f>
         <v>1.7749386396725901</v>
       </c>
       <c r="O7" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" si="6"/>
+        <f>N7/M7</f>
         <v>1.0444736876848677</v>
       </c>
       <c r="Q7" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R7" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I7&gt;K7,1-_xlfn.NORM.DIST(I7,K7,M7,1),_xlfn.NORM.DIST(I7,K7,M7,1))</f>
         <v>0.1481331433566947</v>
       </c>
       <c r="S7" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T7" s="6">
-        <f t="shared" si="10"/>
+        <f>E7/K7</f>
         <v>244.95657965397558</v>
       </c>
       <c r="U7" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C7=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T7)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V7" s="4"/>
@@ -3698,22 +3698,22 @@
       </c>
       <c r="D8" s="4">
         <f t="array" ref="D8">MAX(IF(Sales!B:B=A8,Sales!C:C))</f>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <f>SUMIF(Sales!B:B,A8,Sales!E:E)</f>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G8" s="4">
         <f>SUMIF(Sales!B:B,A8,Sales!D:D)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I8" s="4">
@@ -3721,51 +3721,51 @@
         <v>2</v>
       </c>
       <c r="J8" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K8" s="5">
         <f>SUMIF(Sales!B:B,A8,Sales!F:F)</f>
-        <v>1.7672698512028924</v>
+        <v>1.3260933806146571</v>
       </c>
       <c r="L8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M8" s="5">
         <f>SQRT(SUMIF(Sales!B:B,A8,Sales!G:G))</f>
-        <v>1.237994068051639</v>
+        <v>1.0672538107751555</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" si="4"/>
-        <v>0.23273014879710763</v>
+        <f>I8-K8</f>
+        <v>0.67390661938534291</v>
       </c>
       <c r="O8" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P8" s="5">
-        <f t="shared" si="6"/>
-        <v>0.18798971239287071</v>
+        <f>N8/M8</f>
+        <v>0.63143988110558147</v>
       </c>
       <c r="Q8" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R8" s="17">
-        <f t="shared" si="8"/>
-        <v>0.42544235786385365</v>
+        <f>IF(I8&gt;K8,1-_xlfn.NORM.DIST(I8,K8,M8,1),_xlfn.NORM.DIST(I8,K8,M8,1))</f>
+        <v>0.26387647326386743</v>
       </c>
       <c r="S8" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T8" s="6">
-        <f t="shared" si="10"/>
-        <v>226.33781690314015</v>
+        <f>E8/K8</f>
+        <v>226.22841225626743</v>
       </c>
       <c r="U8" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C8=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T8)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V8" s="4"/>
@@ -3791,7 +3791,7 @@
         <v>800</v>
       </c>
       <c r="F9" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G9" s="4">
@@ -3799,7 +3799,7 @@
         <v>75</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I9" s="4">
@@ -3807,7 +3807,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K9" s="5">
@@ -3815,7 +3815,7 @@
         <v>3.0883035773743104</v>
       </c>
       <c r="L9" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M9" s="5">
@@ -3823,35 +3823,35 @@
         <v>1.645289709282524</v>
       </c>
       <c r="N9" s="5">
-        <f t="shared" si="4"/>
+        <f>I9-K9</f>
         <v>0.91169642262568962</v>
       </c>
       <c r="O9" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P9" s="5">
-        <f t="shared" si="6"/>
+        <f>N9/M9</f>
         <v>0.55412515952783847</v>
       </c>
       <c r="Q9" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R9" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I9&gt;K9,1-_xlfn.NORM.DIST(I9,K9,M9,1),_xlfn.NORM.DIST(I9,K9,M9,1))</f>
         <v>0.28974659632997213</v>
       </c>
       <c r="S9" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T9" s="6">
-        <f t="shared" si="10"/>
+        <f>E9/K9</f>
         <v>259.04189143224175</v>
       </c>
       <c r="U9" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C9=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T9)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V9" s="4"/>
@@ -3877,7 +3877,7 @@
         <v>2060</v>
       </c>
       <c r="F10" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G10" s="4">
@@ -3885,7 +3885,7 @@
         <v>189</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I10" s="4">
@@ -3893,7 +3893,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K10" s="5">
@@ -3901,7 +3901,7 @@
         <v>8.7731840201125806</v>
       </c>
       <c r="L10" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M10" s="5">
@@ -3909,35 +3909,35 @@
         <v>2.7176050085623271</v>
       </c>
       <c r="N10" s="5">
-        <f t="shared" si="4"/>
+        <f>I10-K10</f>
         <v>-0.77318402011258058</v>
       </c>
       <c r="O10" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P10" s="5">
-        <f t="shared" si="6"/>
+        <f>N10/M10</f>
         <v>-0.28450934469009237</v>
       </c>
       <c r="Q10" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R10" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I10&gt;K10,1-_xlfn.NORM.DIST(I10,K10,M10,1),_xlfn.NORM.DIST(I10,K10,M10,1))</f>
         <v>0.3880100368901796</v>
       </c>
       <c r="S10" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T10" s="6">
-        <f t="shared" si="10"/>
+        <f>E10/K10</f>
         <v>234.80642777780983</v>
       </c>
       <c r="U10" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C10=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T10)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V10" s="4"/>
@@ -3963,7 +3963,7 @@
         <v>720</v>
       </c>
       <c r="F11" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G11" s="4">
@@ -3971,7 +3971,7 @@
         <v>68</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I11" s="4">
@@ -3979,7 +3979,7 @@
         <v>7</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K11" s="5">
@@ -3987,7 +3987,7 @@
         <v>3.2402189600805982</v>
       </c>
       <c r="L11" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M11" s="5">
@@ -3995,35 +3995,35 @@
         <v>1.6903967309717229</v>
       </c>
       <c r="N11" s="5">
-        <f t="shared" si="4"/>
+        <f>I11-K11</f>
         <v>3.7597810399194018</v>
       </c>
       <c r="O11" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P11" s="5">
-        <f t="shared" si="6"/>
+        <f>N11/M11</f>
         <v>2.224200373221318</v>
       </c>
       <c r="Q11" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R11" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I11&gt;K11,1-_xlfn.NORM.DIST(I11,K11,M11,1),_xlfn.NORM.DIST(I11,K11,M11,1))</f>
         <v>1.3067482981361178E-2</v>
       </c>
       <c r="S11" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T11" s="6">
-        <f t="shared" si="10"/>
+        <f>E11/K11</f>
         <v>222.20720539888777</v>
       </c>
       <c r="U11" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C11=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T11)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V11" s="4"/>
@@ -4049,7 +4049,7 @@
         <v>1800</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E12)+1)</f>
         <v>1</v>
       </c>
       <c r="G12" s="4">
@@ -4057,7 +4057,7 @@
         <v>170</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G12)+1)</f>
         <v>1</v>
       </c>
       <c r="I12" s="4">
@@ -4065,7 +4065,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I12)+1)</f>
         <v>1</v>
       </c>
       <c r="K12" s="5">
@@ -4073,7 +4073,7 @@
         <v>7.5541199907867584</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K12)+1)</f>
         <v>1</v>
       </c>
       <c r="M12" s="5">
@@ -4081,35 +4081,35 @@
         <v>2.5856751094821875</v>
       </c>
       <c r="N12" s="5">
-        <f t="shared" si="4"/>
+        <f>I12-K12</f>
         <v>1.4458800092132416</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N12)+1)</f>
         <v>4</v>
       </c>
       <c r="P12" s="5">
-        <f t="shared" si="6"/>
+        <f>N12/M12</f>
         <v>0.55918858634285129</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P12)+1)</f>
         <v>5</v>
       </c>
       <c r="R12" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I12&gt;K12,1-_xlfn.NORM.DIST(I12,K12,M12,1),_xlfn.NORM.DIST(I12,K12,M12,1))</f>
         <v>0.28801651091050329</v>
       </c>
       <c r="S12" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R12)+1)</f>
         <v>16</v>
       </c>
       <c r="T12" s="6">
-        <f t="shared" si="10"/>
+        <f>E12/K12</f>
         <v>238.28056771607234</v>
       </c>
       <c r="U12" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C12=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T12)+1)</f>
         <v>20</v>
       </c>
       <c r="V12" s="4"/>
@@ -4135,7 +4135,7 @@
         <v>560</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E13)+1)</f>
         <v>14</v>
       </c>
       <c r="G13" s="4">
@@ -4143,7 +4143,7 @@
         <v>49</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G13)+1)</f>
         <v>15</v>
       </c>
       <c r="I13" s="4">
@@ -4151,7 +4151,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I13)+1)</f>
         <v>23</v>
       </c>
       <c r="K13" s="5">
@@ -4159,7 +4159,7 @@
         <v>2.4986609374725086</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K13)+1)</f>
         <v>14</v>
       </c>
       <c r="M13" s="5">
@@ -4167,35 +4167,35 @@
         <v>1.4954768990915936</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" si="4"/>
+        <f>I13-K13</f>
         <v>-2.4986609374725086</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N13)+1)</f>
         <v>32</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" si="6"/>
+        <f>N13/M13</f>
         <v>-1.6708121262122371</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P13)+1)</f>
         <v>33</v>
       </c>
       <c r="R13" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I13&gt;K13,1-_xlfn.NORM.DIST(I13,K13,M13,1),_xlfn.NORM.DIST(I13,K13,M13,1))</f>
         <v>4.7379396299877204E-2</v>
       </c>
       <c r="S13" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R13)+1)</f>
         <v>32</v>
       </c>
       <c r="T13" s="6">
-        <f t="shared" si="10"/>
+        <f>E13/K13</f>
         <v>224.12004430119339</v>
       </c>
       <c r="U13" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C13=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T13)+1)</f>
         <v>14</v>
       </c>
       <c r="V13" s="4"/>
@@ -4221,7 +4221,7 @@
         <v>530</v>
       </c>
       <c r="F14" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G14" s="4">
@@ -4229,7 +4229,7 @@
         <v>48</v>
       </c>
       <c r="H14" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I14" s="4">
@@ -4237,7 +4237,7 @@
         <v>3</v>
       </c>
       <c r="J14" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K14" s="5">
@@ -4245,7 +4245,7 @@
         <v>2.1645166106756251</v>
       </c>
       <c r="L14" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M14" s="5">
@@ -4253,35 +4253,35 @@
         <v>1.3966272062273601</v>
       </c>
       <c r="N14" s="5">
-        <f t="shared" si="4"/>
+        <f>I14-K14</f>
         <v>0.83548338932437494</v>
       </c>
       <c r="O14" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P14" s="5">
-        <f t="shared" si="6"/>
+        <f>N14/M14</f>
         <v>0.59821503232865181</v>
       </c>
       <c r="Q14" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R14" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I14&gt;K14,1-_xlfn.NORM.DIST(I14,K14,M14,1),_xlfn.NORM.DIST(I14,K14,M14,1))</f>
         <v>0.27484823119819857</v>
       </c>
       <c r="S14" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T14" s="6">
-        <f t="shared" si="10"/>
+        <f>E14/K14</f>
         <v>244.85836578291148</v>
       </c>
       <c r="U14" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C14=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T14)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V14" s="4"/>
@@ -4307,7 +4307,7 @@
         <v>720</v>
       </c>
       <c r="F15" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G15" s="4">
@@ -4315,7 +4315,7 @@
         <v>68</v>
       </c>
       <c r="H15" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I15" s="4">
@@ -4323,7 +4323,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K15" s="5">
@@ -4331,7 +4331,7 @@
         <v>3.3228848135790381</v>
       </c>
       <c r="L15" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M15" s="5">
@@ -4339,35 +4339,35 @@
         <v>1.7072968480631159</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" si="4"/>
+        <f>I15-K15</f>
         <v>-0.32288481357903809</v>
       </c>
       <c r="O15" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="6"/>
+        <f>N15/M15</f>
         <v>-0.18912048830017028</v>
       </c>
       <c r="Q15" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R15" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I15&gt;K15,1-_xlfn.NORM.DIST(I15,K15,M15,1),_xlfn.NORM.DIST(I15,K15,M15,1))</f>
         <v>0.42499919195049596</v>
       </c>
       <c r="S15" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T15" s="6">
-        <f t="shared" si="10"/>
+        <f>E15/K15</f>
         <v>216.67919304867414</v>
       </c>
       <c r="U15" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C15=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T15)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V15" s="4"/>
@@ -4393,7 +4393,7 @@
         <v>1020</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E16)+1)</f>
         <v>5</v>
       </c>
       <c r="G16" s="4">
@@ -4401,7 +4401,7 @@
         <v>98</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G16)+1)</f>
         <v>5</v>
       </c>
       <c r="I16" s="4">
@@ -4409,7 +4409,7 @@
         <v>7</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I16)+1)</f>
         <v>2</v>
       </c>
       <c r="K16" s="5">
@@ -4417,7 +4417,7 @@
         <v>4.5559227870088854</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K16)+1)</f>
         <v>5</v>
       </c>
       <c r="M16" s="5">
@@ -4425,35 +4425,35 @@
         <v>2.0169102529019636</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" si="4"/>
+        <f>I16-K16</f>
         <v>2.4440772129911146</v>
       </c>
       <c r="O16" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N16)+1)</f>
         <v>1</v>
       </c>
       <c r="P16" s="5">
-        <f t="shared" si="6"/>
+        <f>N16/M16</f>
         <v>1.2117927455991342</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P16)+1)</f>
         <v>2</v>
       </c>
       <c r="R16" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I16&gt;K16,1-_xlfn.NORM.DIST(I16,K16,M16,1),_xlfn.NORM.DIST(I16,K16,M16,1))</f>
         <v>0.11279586296928212</v>
       </c>
       <c r="S16" s="32">
-        <f t="shared" si="9"/>
-        <v>30</v>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R16)+1)</f>
+        <v>29</v>
       </c>
       <c r="T16" s="6">
-        <f t="shared" si="10"/>
+        <f>E16/K16</f>
         <v>223.88439130454708</v>
       </c>
       <c r="U16" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C16=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T16)+1)</f>
         <v>13</v>
       </c>
       <c r="V16" s="4"/>
@@ -4479,7 +4479,7 @@
         <v>1040</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E17)+1)</f>
         <v>4</v>
       </c>
       <c r="G17" s="4">
@@ -4487,7 +4487,7 @@
         <v>94</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G17)+1)</f>
         <v>6</v>
       </c>
       <c r="I17" s="4">
@@ -4495,7 +4495,7 @@
         <v>6</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I17)+1)</f>
         <v>3</v>
       </c>
       <c r="K17" s="5">
@@ -4503,7 +4503,7 @@
         <v>4.8974107512412388</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K17)+1)</f>
         <v>4</v>
       </c>
       <c r="M17" s="5">
@@ -4511,35 +4511,35 @@
         <v>2.0850751321114935</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="4"/>
+        <f>I17-K17</f>
         <v>1.1025892487587612</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N17)+1)</f>
         <v>6</v>
       </c>
       <c r="P17" s="5">
-        <f t="shared" si="6"/>
+        <f>N17/M17</f>
         <v>0.52880072846209714</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P17)+1)</f>
         <v>7</v>
       </c>
       <c r="R17" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I17&gt;K17,1-_xlfn.NORM.DIST(I17,K17,M17,1),_xlfn.NORM.DIST(I17,K17,M17,1))</f>
         <v>0.29847184618231593</v>
       </c>
       <c r="S17" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R17)+1)</f>
         <v>14</v>
       </c>
       <c r="T17" s="6">
-        <f t="shared" si="10"/>
+        <f>E17/K17</f>
         <v>212.35711130344012</v>
       </c>
       <c r="U17" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C17=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T17)+1)</f>
         <v>7</v>
       </c>
       <c r="V17" s="4"/>
@@ -4565,7 +4565,7 @@
         <v>220</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E18)+1)</f>
         <v>24</v>
       </c>
       <c r="G18" s="4">
@@ -4573,7 +4573,7 @@
         <v>19</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G18)+1)</f>
         <v>24</v>
       </c>
       <c r="I18" s="4">
@@ -4581,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I18)+1)</f>
         <v>23</v>
       </c>
       <c r="K18" s="5">
@@ -4589,7 +4589,7 @@
         <v>0.88919799389614118</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K18)+1)</f>
         <v>24</v>
       </c>
       <c r="M18" s="5">
@@ -4597,35 +4597,35 @@
         <v>0.90983539619619269</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="4"/>
+        <f>I18-K18</f>
         <v>-0.88919799389614118</v>
       </c>
       <c r="O18" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N18)+1)</f>
         <v>25</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" si="6"/>
+        <f>N18/M18</f>
         <v>-0.97731743303642438</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P18)+1)</f>
         <v>28</v>
       </c>
       <c r="R18" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I18&gt;K18,1-_xlfn.NORM.DIST(I18,K18,M18,1),_xlfn.NORM.DIST(I18,K18,M18,1))</f>
         <v>0.16420601256102682</v>
       </c>
       <c r="S18" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R18)+1)</f>
         <v>25</v>
       </c>
       <c r="T18" s="6">
-        <f t="shared" si="10"/>
+        <f>E18/K18</f>
         <v>247.41396349314766</v>
       </c>
       <c r="U18" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C18=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T18)+1)</f>
         <v>26</v>
       </c>
       <c r="V18" s="4"/>
@@ -4651,23 +4651,23 @@
         <v>340</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E19)+1)</f>
+        <v>20</v>
       </c>
       <c r="G19" s="4">
         <f>SUMIF(Sales!B:B,A19,Sales!D:D)</f>
         <v>32</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G19)+1)</f>
+        <v>19</v>
       </c>
       <c r="I19" s="4">
         <f>SUMIF(Prizes!B:B,A19,Prizes!D:D)</f>
         <v>1</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I19)+1)</f>
         <v>18</v>
       </c>
       <c r="K19" s="5">
@@ -4675,43 +4675,43 @@
         <v>1.3786580188649971</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="3"/>
-        <v>21</v>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K19)+1)</f>
+        <v>22</v>
       </c>
       <c r="M19" s="5">
         <f>SQRT(SUMIF(Sales!B:B,A19,Sales!G:G))</f>
         <v>1.1321394309179194</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="4"/>
+        <f>I19-K19</f>
         <v>-0.37865801886499706</v>
       </c>
       <c r="O19" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N19)+1)</f>
         <v>18</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" si="6"/>
+        <f>N19/M19</f>
         <v>-0.33446235377385236</v>
       </c>
       <c r="Q19" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P19)+1)</f>
         <v>16</v>
       </c>
       <c r="R19" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I19&gt;K19,1-_xlfn.NORM.DIST(I19,K19,M19,1),_xlfn.NORM.DIST(I19,K19,M19,1))</f>
         <v>0.36901534705848416</v>
       </c>
       <c r="S19" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R19)+1)</f>
         <v>8</v>
       </c>
       <c r="T19" s="6">
-        <f t="shared" si="10"/>
+        <f>E19/K19</f>
         <v>246.61663396402727</v>
       </c>
       <c r="U19" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C19=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T19)+1)</f>
         <v>24</v>
       </c>
       <c r="V19" s="4"/>
@@ -4737,7 +4737,7 @@
         <v>150</v>
       </c>
       <c r="F20" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G20" s="4">
@@ -4745,7 +4745,7 @@
         <v>11</v>
       </c>
       <c r="H20" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I20" s="4">
@@ -4753,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K20" s="5">
@@ -4761,7 +4761,7 @@
         <v>0.70284369885433717</v>
       </c>
       <c r="L20" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M20" s="5">
@@ -4769,35 +4769,35 @@
         <v>0.78059289122728581</v>
       </c>
       <c r="N20" s="5">
-        <f t="shared" si="4"/>
+        <f>I20-K20</f>
         <v>0.29715630114566283</v>
       </c>
       <c r="O20" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P20" s="5">
-        <f t="shared" si="6"/>
+        <f>N20/M20</f>
         <v>0.38068025533573507</v>
       </c>
       <c r="Q20" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R20" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I20&gt;K20,1-_xlfn.NORM.DIST(I20,K20,M20,1),_xlfn.NORM.DIST(I20,K20,M20,1))</f>
         <v>0.35172026081826924</v>
       </c>
       <c r="S20" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T20" s="6">
-        <f t="shared" si="10"/>
+        <f>E20/K20</f>
         <v>213.41871634405473</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C20=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T20)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V20" s="4"/>
@@ -4823,7 +4823,7 @@
         <v>1570</v>
       </c>
       <c r="F21" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G21" s="4">
@@ -4831,7 +4831,7 @@
         <v>147</v>
       </c>
       <c r="H21" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I21" s="4">
@@ -4839,7 +4839,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K21" s="5">
@@ -4847,7 +4847,7 @@
         <v>5.3872370398255942</v>
       </c>
       <c r="L21" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M21" s="5">
@@ -4855,35 +4855,35 @@
         <v>2.1480307909963821</v>
       </c>
       <c r="N21" s="5">
-        <f t="shared" si="4"/>
+        <f>I21-K21</f>
         <v>-1.3872370398255942</v>
       </c>
       <c r="O21" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P21" s="5">
-        <f t="shared" si="6"/>
+        <f>N21/M21</f>
         <v>-0.6458180421064228</v>
       </c>
       <c r="Q21" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R21" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I21&gt;K21,1-_xlfn.NORM.DIST(I21,K21,M21,1),_xlfn.NORM.DIST(I21,K21,M21,1))</f>
         <v>0.25919860106105741</v>
       </c>
       <c r="S21" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" si="10"/>
+        <f>E21/K21</f>
         <v>291.4295377006145</v>
       </c>
       <c r="U21" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C21=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T21)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V21" s="4"/>
@@ -4909,7 +4909,7 @@
         <v>860</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E22)+1)</f>
         <v>7</v>
       </c>
       <c r="G22" s="4">
@@ -4917,7 +4917,7 @@
         <v>85</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G22)+1)</f>
         <v>7</v>
       </c>
       <c r="I22" s="4">
@@ -4925,7 +4925,7 @@
         <v>6</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I22)+1)</f>
         <v>3</v>
       </c>
       <c r="K22" s="5">
@@ -4933,7 +4933,7 @@
         <v>3.8059384171605499</v>
       </c>
       <c r="L22" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K22)+1)</f>
         <v>7</v>
       </c>
       <c r="M22" s="5">
@@ -4941,35 +4941,35 @@
         <v>1.8697596112891726</v>
       </c>
       <c r="N22" s="5">
-        <f t="shared" si="4"/>
+        <f>I22-K22</f>
         <v>2.1940615828394501</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N22)+1)</f>
         <v>3</v>
       </c>
       <c r="P22" s="5">
-        <f t="shared" si="6"/>
+        <f>N22/M22</f>
         <v>1.1734458106765264</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P22)+1)</f>
         <v>3</v>
       </c>
       <c r="R22" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I22&gt;K22,1-_xlfn.NORM.DIST(I22,K22,M22,1),_xlfn.NORM.DIST(I22,K22,M22,1))</f>
         <v>0.12030853778064177</v>
       </c>
       <c r="S22" s="32">
-        <f t="shared" si="9"/>
-        <v>29</v>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R22)+1)</f>
+        <v>28</v>
       </c>
       <c r="T22" s="6">
-        <f t="shared" si="10"/>
+        <f>E22/K22</f>
         <v>225.96266826661102</v>
       </c>
       <c r="U22" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C22=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T22)+1)</f>
         <v>16</v>
       </c>
       <c r="V22" s="4"/>
@@ -4995,7 +4995,7 @@
         <v>200</v>
       </c>
       <c r="F23" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G23" s="4">
@@ -5003,7 +5003,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I23" s="4">
@@ -5011,7 +5011,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K23" s="5">
@@ -5019,7 +5019,7 @@
         <v>0.63164893617021267</v>
       </c>
       <c r="L23" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M23" s="5">
@@ -5027,35 +5027,35 @@
         <v>0.75810728959235163</v>
       </c>
       <c r="N23" s="5">
-        <f t="shared" si="4"/>
+        <f>I23-K23</f>
         <v>0.36835106382978733</v>
       </c>
       <c r="O23" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P23" s="5">
-        <f t="shared" si="6"/>
+        <f>N23/M23</f>
         <v>0.4858824982778579</v>
       </c>
       <c r="Q23" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R23" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I23&gt;K23,1-_xlfn.NORM.DIST(I23,K23,M23,1),_xlfn.NORM.DIST(I23,K23,M23,1))</f>
         <v>0.31352523895390516</v>
       </c>
       <c r="S23" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" si="10"/>
+        <f>E23/K23</f>
         <v>316.6315789473685</v>
       </c>
       <c r="U23" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C23=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T23)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V23" s="4"/>
@@ -5081,7 +5081,7 @@
         <v>100</v>
       </c>
       <c r="F24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G24" s="4">
@@ -5089,7 +5089,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I24" s="4">
@@ -5097,7 +5097,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K24" s="5">
@@ -5105,7 +5105,7 @@
         <v>0.54326923076923084</v>
       </c>
       <c r="L24" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M24" s="5">
@@ -5113,35 +5113,35 @@
         <v>0.67686632105875888</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="4"/>
+        <f>I24-K24</f>
         <v>0.45673076923076916</v>
       </c>
       <c r="O24" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P24" s="5">
-        <f t="shared" si="6"/>
+        <f>N24/M24</f>
         <v>0.67477248464120332</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R24" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I24&gt;K24,1-_xlfn.NORM.DIST(I24,K24,M24,1),_xlfn.NORM.DIST(I24,K24,M24,1))</f>
         <v>0.24991016218462114</v>
       </c>
       <c r="S24" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T24" s="6">
-        <f t="shared" si="10"/>
+        <f>E24/K24</f>
         <v>184.07079646017698</v>
       </c>
       <c r="U24" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C24=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T24)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V24" s="4"/>
@@ -5167,7 +5167,7 @@
         <v>800</v>
       </c>
       <c r="F25" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G25" s="4">
@@ -5175,7 +5175,7 @@
         <v>75</v>
       </c>
       <c r="H25" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I25" s="4">
@@ -5183,7 +5183,7 @@
         <v>4</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K25" s="5">
@@ -5191,7 +5191,7 @@
         <v>2.9991021425331783</v>
       </c>
       <c r="L25" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M25" s="5">
@@ -5199,35 +5199,35 @@
         <v>1.640793642686911</v>
       </c>
       <c r="N25" s="5">
-        <f t="shared" si="4"/>
+        <f>I25-K25</f>
         <v>1.0008978574668217</v>
       </c>
       <c r="O25" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P25" s="5">
-        <f t="shared" si="6"/>
+        <f>N25/M25</f>
         <v>0.61000837120979057</v>
       </c>
       <c r="Q25" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R25" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I25&gt;K25,1-_xlfn.NORM.DIST(I25,K25,M25,1),_xlfn.NORM.DIST(I25,K25,M25,1))</f>
         <v>0.27092813112251135</v>
       </c>
       <c r="S25" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" si="10"/>
+        <f>E25/K25</f>
         <v>266.74650011229147</v>
       </c>
       <c r="U25" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C25=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T25)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V25" s="4"/>
@@ -5253,7 +5253,7 @@
         <v>850</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E26)+1)</f>
         <v>8</v>
       </c>
       <c r="G26" s="4">
@@ -5261,7 +5261,7 @@
         <v>81</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G26)+1)</f>
         <v>9</v>
       </c>
       <c r="I26" s="4">
@@ -5269,7 +5269,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I26)+1)</f>
         <v>18</v>
       </c>
       <c r="K26" s="5">
@@ -5277,7 +5277,7 @@
         <v>3.4203082743728253</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K26)+1)</f>
         <v>8</v>
       </c>
       <c r="M26" s="5">
@@ -5285,35 +5285,35 @@
         <v>1.7553836370630092</v>
       </c>
       <c r="N26" s="5">
-        <f t="shared" si="4"/>
+        <f>I26-K26</f>
         <v>-2.4203082743728253</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N26)+1)</f>
         <v>31</v>
       </c>
       <c r="P26" s="5">
-        <f t="shared" si="6"/>
+        <f>N26/M26</f>
         <v>-1.3787916346436517</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P26)+1)</f>
         <v>32</v>
       </c>
       <c r="R26" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I26&gt;K26,1-_xlfn.NORM.DIST(I26,K26,M26,1),_xlfn.NORM.DIST(I26,K26,M26,1))</f>
         <v>8.3979503335431097E-2</v>
       </c>
       <c r="S26" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R26)+1)</f>
         <v>31</v>
       </c>
       <c r="T26" s="6">
-        <f t="shared" si="10"/>
+        <f>E26/K26</f>
         <v>248.51561082044944</v>
       </c>
       <c r="U26" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C26=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T26)+1)</f>
         <v>27</v>
       </c>
       <c r="V26" s="4"/>
@@ -5339,7 +5339,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G27" s="4">
@@ -5347,7 +5347,7 @@
         <v>2</v>
       </c>
       <c r="H27" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I27" s="4">
@@ -5355,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K27" s="5">
@@ -5363,7 +5363,7 @@
         <v>6.3829787234042548E-2</v>
       </c>
       <c r="L27" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M27" s="5">
@@ -5371,35 +5371,35 @@
         <v>0.24791576048881739</v>
       </c>
       <c r="N27" s="5">
-        <f t="shared" si="4"/>
+        <f>I27-K27</f>
         <v>-6.3829787234042548E-2</v>
       </c>
       <c r="O27" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P27" s="5">
-        <f t="shared" si="6"/>
+        <f>N27/M27</f>
         <v>-0.25746562908380199</v>
       </c>
       <c r="Q27" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R27" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I27&gt;K27,1-_xlfn.NORM.DIST(I27,K27,M27,1),_xlfn.NORM.DIST(I27,K27,M27,1))</f>
         <v>0.39840967257938792</v>
       </c>
       <c r="S27" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T27" s="6">
-        <f t="shared" si="10"/>
+        <f>E27/K27</f>
         <v>313.33333333333337</v>
       </c>
       <c r="U27" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C27=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T27)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V27" s="4"/>
@@ -5425,7 +5425,7 @@
         <v>100</v>
       </c>
       <c r="F28" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G28" s="4">
@@ -5433,7 +5433,7 @@
         <v>10</v>
       </c>
       <c r="H28" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I28" s="4">
@@ -5441,7 +5441,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K28" s="5">
@@ -5449,7 +5449,7 @@
         <v>0.31914893617021273</v>
       </c>
       <c r="L28" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M28" s="5">
@@ -5457,35 +5457,35 @@
         <v>0.54230382522055953</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="4"/>
+        <f>I28-K28</f>
         <v>-0.31914893617021273</v>
       </c>
       <c r="O28" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P28" s="5">
-        <f t="shared" si="6"/>
+        <f>N28/M28</f>
         <v>-0.58850578094375816</v>
       </c>
       <c r="Q28" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R28" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I28&gt;K28,1-_xlfn.NORM.DIST(I28,K28,M28,1),_xlfn.NORM.DIST(I28,K28,M28,1))</f>
         <v>0.27809642736849838</v>
       </c>
       <c r="S28" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T28" s="6">
-        <f t="shared" si="10"/>
+        <f>E28/K28</f>
         <v>313.33333333333337</v>
       </c>
       <c r="U28" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C28=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T28)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V28" s="4"/>
@@ -5511,7 +5511,7 @@
         <v>100</v>
       </c>
       <c r="F29" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G29" s="4">
@@ -5519,7 +5519,7 @@
         <v>11</v>
       </c>
       <c r="H29" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I29" s="4">
@@ -5527,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K29" s="5">
@@ -5535,7 +5535,7 @@
         <v>0.58616138763197578</v>
       </c>
       <c r="L29" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M29" s="5">
@@ -5543,35 +5543,35 @@
         <v>0.71401106976234563</v>
       </c>
       <c r="N29" s="5">
-        <f t="shared" si="4"/>
+        <f>I29-K29</f>
         <v>-0.58616138763197578</v>
       </c>
       <c r="O29" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P29" s="5">
-        <f t="shared" si="6"/>
+        <f>N29/M29</f>
         <v>-0.82094159664369926</v>
       </c>
       <c r="Q29" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R29" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I29&gt;K29,1-_xlfn.NORM.DIST(I29,K29,M29,1),_xlfn.NORM.DIST(I29,K29,M29,1))</f>
         <v>0.20583976793322406</v>
       </c>
       <c r="S29" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T29" s="6">
-        <f t="shared" si="10"/>
+        <f>E29/K29</f>
         <v>170.6014795754262</v>
       </c>
       <c r="U29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C29=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T29)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V29" s="4"/>
@@ -5597,7 +5597,7 @@
         <v>240</v>
       </c>
       <c r="F30" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G30" s="4">
@@ -5605,7 +5605,7 @@
         <v>24</v>
       </c>
       <c r="H30" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I30" s="4">
@@ -5613,7 +5613,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K30" s="5">
@@ -5621,7 +5621,7 @@
         <v>0.7941427895328429</v>
       </c>
       <c r="L30" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M30" s="5">
@@ -5629,35 +5629,35 @@
         <v>0.86060092285446455</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" si="4"/>
+        <f>I30-K30</f>
         <v>-0.7941427895328429</v>
       </c>
       <c r="O30" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P30" s="5">
-        <f t="shared" si="6"/>
+        <f>N30/M30</f>
         <v>-0.92277706012539296</v>
       </c>
       <c r="Q30" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R30" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I30&gt;K30,1-_xlfn.NORM.DIST(I30,K30,M30,1),_xlfn.NORM.DIST(I30,K30,M30,1))</f>
         <v>0.17806169891377793</v>
       </c>
       <c r="S30" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T30" s="6">
-        <f t="shared" si="10"/>
+        <f>E30/K30</f>
         <v>302.21265389966049</v>
       </c>
       <c r="U30" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C30=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T30)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V30" s="4"/>
@@ -5683,7 +5683,7 @@
         <v>1000</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" si="0"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E31)+1)</f>
         <v>6</v>
       </c>
       <c r="G31" s="4">
@@ -5691,7 +5691,7 @@
         <v>101</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="1"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G31)+1)</f>
         <v>4</v>
       </c>
       <c r="I31" s="4">
@@ -5699,7 +5699,7 @@
         <v>4</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="2"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I31)+1)</f>
         <v>6</v>
       </c>
       <c r="K31" s="5">
@@ -5707,7 +5707,7 @@
         <v>4.1786525121430946</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="3"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K31)+1)</f>
         <v>6</v>
       </c>
       <c r="M31" s="5">
@@ -5715,35 +5715,35 @@
         <v>1.9324236475762098</v>
       </c>
       <c r="N31" s="5">
-        <f t="shared" si="4"/>
+        <f>I31-K31</f>
         <v>-0.17865251214309463</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" si="5"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N31)+1)</f>
         <v>16</v>
       </c>
       <c r="P31" s="5">
-        <f t="shared" si="6"/>
+        <f>N31/M31</f>
         <v>-9.2449972016836982E-2</v>
       </c>
       <c r="Q31" s="4">
-        <f t="shared" si="7"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P31)+1)</f>
         <v>12</v>
       </c>
       <c r="R31" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I31&gt;K31,1-_xlfn.NORM.DIST(I31,K31,M31,1),_xlfn.NORM.DIST(I31,K31,M31,1))</f>
         <v>0.46317026873308886</v>
       </c>
       <c r="S31" s="32">
-        <f t="shared" si="9"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R31)+1)</f>
         <v>1</v>
       </c>
       <c r="T31" s="6">
-        <f t="shared" si="10"/>
+        <f>E31/K31</f>
         <v>239.31159556675667</v>
       </c>
       <c r="U31" s="4">
-        <f t="shared" si="11"/>
+        <f>IF($C31=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T31)+1)</f>
         <v>21</v>
       </c>
       <c r="V31" s="4"/>
@@ -5769,7 +5769,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G32" s="4">
@@ -5777,7 +5777,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I32" s="4">
@@ -5785,7 +5785,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K32" s="5">
@@ -5793,7 +5793,7 @@
         <v>0.20833333333333331</v>
       </c>
       <c r="L32" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M32" s="5">
@@ -5801,35 +5801,35 @@
         <v>0.43925136315935126</v>
       </c>
       <c r="N32" s="5">
-        <f t="shared" si="4"/>
+        <f>I32-K32</f>
         <v>-0.20833333333333331</v>
       </c>
       <c r="O32" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" si="6"/>
+        <f>N32/M32</f>
         <v>-0.47429183107111794</v>
       </c>
       <c r="Q32" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R32" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I32&gt;K32,1-_xlfn.NORM.DIST(I32,K32,M32,1),_xlfn.NORM.DIST(I32,K32,M32,1))</f>
         <v>0.31764590799841352</v>
       </c>
       <c r="S32" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T32" s="6">
-        <f t="shared" si="10"/>
+        <f>E32/K32</f>
         <v>240.00000000000003</v>
       </c>
       <c r="U32" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C32=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T32)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V32" s="4"/>
@@ -5855,7 +5855,7 @@
         <v>160</v>
       </c>
       <c r="F33" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G33" s="4">
@@ -5863,7 +5863,7 @@
         <v>16</v>
       </c>
       <c r="H33" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I33" s="4">
@@ -5871,7 +5871,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K33" s="5">
@@ -5879,7 +5879,7 @@
         <v>0.68315789473684219</v>
       </c>
       <c r="L33" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M33" s="5">
@@ -5887,35 +5887,35 @@
         <v>0.79496113990168826</v>
       </c>
       <c r="N33" s="5">
-        <f t="shared" si="4"/>
+        <f>I33-K33</f>
         <v>0.31684210526315781</v>
       </c>
       <c r="O33" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P33" s="5">
-        <f t="shared" si="6"/>
+        <f>N33/M33</f>
         <v>0.39856301064268529</v>
       </c>
       <c r="Q33" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R33" s="17">
-        <f t="shared" si="8"/>
+        <f>IF(I33&gt;K33,1-_xlfn.NORM.DIST(I33,K33,M33,1),_xlfn.NORM.DIST(I33,K33,M33,1))</f>
         <v>0.34510761059987882</v>
       </c>
       <c r="S33" s="32" t="str">
-        <f t="shared" si="9"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T33" s="6">
-        <f t="shared" si="10"/>
+        <f>E33/K33</f>
         <v>234.20647149460706</v>
       </c>
       <c r="U33" s="6" t="str">
-        <f t="shared" si="11"/>
+        <f>IF($C33=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T33)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V33" s="4"/>
@@ -5941,7 +5941,7 @@
         <v>820</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" ref="F34:F52" si="12">IF($C34=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E34)+1)</f>
         <v>9</v>
       </c>
       <c r="G34" s="4">
@@ -5949,7 +5949,7 @@
         <v>83</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" ref="H34:H52" si="13">IF($C34=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G34)+1)</f>
         <v>8</v>
       </c>
       <c r="I34" s="4">
@@ -5957,7 +5957,7 @@
         <v>4</v>
       </c>
       <c r="J34" s="4">
-        <f t="shared" ref="J34:J52" si="14">IF($C34=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I34)+1)</f>
         <v>6</v>
       </c>
       <c r="K34" s="5">
@@ -5965,7 +5965,7 @@
         <v>3.4054149521089765</v>
       </c>
       <c r="L34" s="6">
-        <f t="shared" ref="L34:L52" si="15">IF($C34=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K34)+1)</f>
         <v>9</v>
       </c>
       <c r="M34" s="5">
@@ -5973,35 +5973,35 @@
         <v>1.7445127563867142</v>
       </c>
       <c r="N34" s="5">
-        <f t="shared" ref="N34:N52" si="16">I34-K34</f>
+        <f>I34-K34</f>
         <v>0.59458504789102351</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" ref="O34:O52" si="17">IF($C34=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N34)+1)</f>
         <v>8</v>
       </c>
       <c r="P34" s="5">
-        <f t="shared" ref="P34:P52" si="18">N34/M34</f>
+        <f>N34/M34</f>
         <v>0.34083158504529681</v>
       </c>
       <c r="Q34" s="4">
-        <f t="shared" ref="Q34:Q52" si="19">IF($C34=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P34)+1)</f>
         <v>8</v>
       </c>
       <c r="R34" s="17">
-        <f t="shared" ref="R34:R52" si="20">IF(I34&gt;K34,1-_xlfn.NORM.DIST(I34,K34,M34,1),_xlfn.NORM.DIST(I34,K34,M34,1))</f>
+        <f>IF(I34&gt;K34,1-_xlfn.NORM.DIST(I34,K34,M34,1),_xlfn.NORM.DIST(I34,K34,M34,1))</f>
         <v>0.36661518558908524</v>
       </c>
       <c r="S34" s="32">
-        <f t="shared" ref="S34:S52" si="21">IF($C34=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R34)+1)</f>
         <v>9</v>
       </c>
       <c r="T34" s="6">
-        <f t="shared" ref="T34:T52" si="22">E34/K34</f>
+        <f>E34/K34</f>
         <v>240.79297575532559</v>
       </c>
       <c r="U34" s="4">
-        <f t="shared" ref="U34:U52" si="23">IF($C34=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T34)+1)</f>
+        <f>IF($C34=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T34)+1)</f>
         <v>22</v>
       </c>
       <c r="V34" s="4"/>
@@ -6027,7 +6027,7 @@
         <v>1510</v>
       </c>
       <c r="F35" s="6">
-        <f t="shared" si="12"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E35)+1)</f>
         <v>2</v>
       </c>
       <c r="G35" s="4">
@@ -6035,7 +6035,7 @@
         <v>152</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="13"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G35)+1)</f>
         <v>2</v>
       </c>
       <c r="I35" s="4">
@@ -6043,7 +6043,7 @@
         <v>6</v>
       </c>
       <c r="J35" s="4">
-        <f t="shared" si="14"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I35)+1)</f>
         <v>3</v>
       </c>
       <c r="K35" s="5">
@@ -6051,7 +6051,7 @@
         <v>6.7593403877425144</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K35)+1)</f>
         <v>2</v>
       </c>
       <c r="M35" s="5">
@@ -6059,35 +6059,35 @@
         <v>2.4375937677521211</v>
       </c>
       <c r="N35" s="5">
-        <f t="shared" si="16"/>
+        <f>I35-K35</f>
         <v>-0.75934038774251444</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="17"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N35)+1)</f>
         <v>23</v>
       </c>
       <c r="P35" s="5">
-        <f t="shared" si="18"/>
+        <f>N35/M35</f>
         <v>-0.31151227812776872</v>
       </c>
       <c r="Q35" s="4">
-        <f t="shared" si="19"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P35)+1)</f>
         <v>15</v>
       </c>
       <c r="R35" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I35&gt;K35,1-_xlfn.NORM.DIST(I35,K35,M35,1),_xlfn.NORM.DIST(I35,K35,M35,1))</f>
         <v>0.37770560515978768</v>
       </c>
       <c r="S35" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R35)+1)</f>
         <v>7</v>
       </c>
       <c r="T35" s="6">
-        <f t="shared" si="22"/>
+        <f>E35/K35</f>
         <v>223.39457896487295</v>
       </c>
       <c r="U35" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C35=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T35)+1)</f>
         <v>12</v>
       </c>
       <c r="V35" s="4"/>
@@ -6113,7 +6113,7 @@
         <v>750</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" si="12"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E36)+1)</f>
         <v>10</v>
       </c>
       <c r="G36" s="4">
@@ -6121,7 +6121,7 @@
         <v>76</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="13"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G36)+1)</f>
         <v>10</v>
       </c>
       <c r="I36" s="4">
@@ -6129,7 +6129,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="4">
-        <f t="shared" si="14"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I36)+1)</f>
         <v>11</v>
       </c>
       <c r="K36" s="5">
@@ -6137,7 +6137,7 @@
         <v>3.3959495602492105</v>
       </c>
       <c r="L36" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K36)+1)</f>
         <v>10</v>
       </c>
       <c r="M36" s="5">
@@ -6145,35 +6145,35 @@
         <v>1.7584640236594731</v>
       </c>
       <c r="N36" s="5">
-        <f t="shared" si="16"/>
+        <f>I36-K36</f>
         <v>-1.3959495602492105</v>
       </c>
       <c r="O36" s="6">
-        <f t="shared" si="17"/>
-        <v>30</v>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N36)+1)</f>
+        <v>29</v>
       </c>
       <c r="P36" s="5">
-        <f t="shared" si="18"/>
+        <f>N36/M36</f>
         <v>-0.79384595958019799</v>
       </c>
       <c r="Q36" s="4">
-        <f t="shared" si="19"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P36)+1)</f>
         <v>27</v>
       </c>
       <c r="R36" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I36&gt;K36,1-_xlfn.NORM.DIST(I36,K36,M36,1),_xlfn.NORM.DIST(I36,K36,M36,1))</f>
         <v>0.21364255652874861</v>
       </c>
       <c r="S36" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R36)+1)</f>
         <v>23</v>
       </c>
       <c r="T36" s="6">
-        <f t="shared" si="22"/>
+        <f>E36/K36</f>
         <v>220.85133677455491</v>
       </c>
       <c r="U36" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C36=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T36)+1)</f>
         <v>10</v>
       </c>
       <c r="V36" s="4"/>
@@ -6199,7 +6199,7 @@
         <v>650</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" si="12"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E37)+1)</f>
         <v>12</v>
       </c>
       <c r="G37" s="4">
@@ -6207,7 +6207,7 @@
         <v>66</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="13"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G37)+1)</f>
         <v>11</v>
       </c>
       <c r="I37" s="4">
@@ -6215,7 +6215,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="14"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I37)+1)</f>
         <v>11</v>
       </c>
       <c r="K37" s="5">
@@ -6223,7 +6223,7 @@
         <v>3.0918110715694103</v>
       </c>
       <c r="L37" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K37)+1)</f>
         <v>11</v>
       </c>
       <c r="M37" s="5">
@@ -6231,35 +6231,35 @@
         <v>1.6769795571951143</v>
       </c>
       <c r="N37" s="5">
-        <f t="shared" si="16"/>
+        <f>I37-K37</f>
         <v>-1.0918110715694103</v>
       </c>
       <c r="O37" s="6">
-        <f t="shared" si="17"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N37)+1)</f>
         <v>27</v>
       </c>
       <c r="P37" s="5">
-        <f t="shared" si="18"/>
+        <f>N37/M37</f>
         <v>-0.65105806858823834</v>
       </c>
       <c r="Q37" s="4">
-        <f t="shared" si="19"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P37)+1)</f>
         <v>22</v>
       </c>
       <c r="R37" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I37&gt;K37,1-_xlfn.NORM.DIST(I37,K37,M37,1),_xlfn.NORM.DIST(I37,K37,M37,1))</f>
         <v>0.25750450144443959</v>
       </c>
       <c r="S37" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R37)+1)</f>
         <v>18</v>
       </c>
       <c r="T37" s="6">
-        <f t="shared" si="22"/>
+        <f>E37/K37</f>
         <v>210.23276809409268</v>
       </c>
       <c r="U37" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C37=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T37)+1)</f>
         <v>4</v>
       </c>
       <c r="V37" s="4"/>
@@ -6285,7 +6285,7 @@
         <v>450</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" si="12"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E38)+1)</f>
         <v>16</v>
       </c>
       <c r="G38" s="4">
@@ -6293,7 +6293,7 @@
         <v>46</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="13"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G38)+1)</f>
         <v>16</v>
       </c>
       <c r="I38" s="4">
@@ -6301,7 +6301,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4">
-        <f t="shared" si="14"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I38)+1)</f>
         <v>11</v>
       </c>
       <c r="K38" s="5">
@@ -6309,7 +6309,7 @@
         <v>2.1354304779193765</v>
       </c>
       <c r="L38" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K38)+1)</f>
         <v>15</v>
       </c>
       <c r="M38" s="5">
@@ -6317,35 +6317,35 @@
         <v>1.3926588531059174</v>
       </c>
       <c r="N38" s="5">
-        <f t="shared" si="16"/>
+        <f>I38-K38</f>
         <v>-0.13543047791937646</v>
       </c>
       <c r="O38" s="6">
-        <f t="shared" si="17"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N38)+1)</f>
         <v>13</v>
       </c>
       <c r="P38" s="5">
-        <f t="shared" si="18"/>
+        <f>N38/M38</f>
         <v>-9.7245982113522256E-2</v>
       </c>
       <c r="Q38" s="4">
-        <f t="shared" si="19"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P38)+1)</f>
         <v>13</v>
       </c>
       <c r="R38" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I38&gt;K38,1-_xlfn.NORM.DIST(I38,K38,M38,1),_xlfn.NORM.DIST(I38,K38,M38,1))</f>
         <v>0.46126552630700979</v>
       </c>
       <c r="S38" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R38)+1)</f>
         <v>2</v>
       </c>
       <c r="T38" s="6">
-        <f t="shared" si="22"/>
+        <f>E38/K38</f>
         <v>210.73034437461553</v>
       </c>
       <c r="U38" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C38=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T38)+1)</f>
         <v>5</v>
       </c>
       <c r="V38" s="4"/>
@@ -6371,7 +6371,7 @@
         <v>1500</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="12"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E39)+1)</f>
         <v>3</v>
       </c>
       <c r="G39" s="4">
@@ -6379,7 +6379,7 @@
         <v>151</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="13"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G39)+1)</f>
         <v>3</v>
       </c>
       <c r="I39" s="4">
@@ -6387,7 +6387,7 @@
         <v>4</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="14"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I39)+1)</f>
         <v>6</v>
       </c>
       <c r="K39" s="5">
@@ -6395,7 +6395,7 @@
         <v>6.7456182608128401</v>
       </c>
       <c r="L39" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K39)+1)</f>
         <v>3</v>
       </c>
       <c r="M39" s="5">
@@ -6403,35 +6403,35 @@
         <v>2.4361086141088233</v>
       </c>
       <c r="N39" s="5">
-        <f t="shared" si="16"/>
+        <f>I39-K39</f>
         <v>-2.7456182608128401</v>
       </c>
       <c r="O39" s="6">
-        <f t="shared" si="17"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N39)+1)</f>
         <v>33</v>
       </c>
       <c r="P39" s="5">
-        <f t="shared" si="18"/>
+        <f>N39/M39</f>
         <v>-1.1270508403900708</v>
       </c>
       <c r="Q39" s="4">
-        <f t="shared" si="19"/>
-        <v>30</v>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P39)+1)</f>
+        <v>29</v>
       </c>
       <c r="R39" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I39&gt;K39,1-_xlfn.NORM.DIST(I39,K39,M39,1),_xlfn.NORM.DIST(I39,K39,M39,1))</f>
         <v>0.12986049313998585</v>
       </c>
       <c r="S39" s="32">
-        <f t="shared" si="21"/>
-        <v>27</v>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R39)+1)</f>
+        <v>26</v>
       </c>
       <c r="T39" s="6">
-        <f t="shared" si="22"/>
+        <f>E39/K39</f>
         <v>222.3665707136015</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C39=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T39)+1)</f>
         <v>11</v>
       </c>
       <c r="V39" s="4"/>
@@ -6457,7 +6457,7 @@
         <v>360</v>
       </c>
       <c r="F40" s="30" t="str">
-        <f t="shared" si="12"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G40" s="8">
@@ -6465,7 +6465,7 @@
         <v>37</v>
       </c>
       <c r="H40" s="8" t="str">
-        <f t="shared" si="13"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I40" s="8">
@@ -6473,7 +6473,7 @@
         <v>4</v>
       </c>
       <c r="J40" s="8" t="str">
-        <f t="shared" si="14"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K40" s="9">
@@ -6481,7 +6481,7 @@
         <v>1.7654362892118982</v>
       </c>
       <c r="L40" s="30" t="str">
-        <f t="shared" si="15"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M40" s="9">
@@ -6489,35 +6489,35 @@
         <v>1.2439598119364987</v>
       </c>
       <c r="N40" s="9">
-        <f t="shared" si="16"/>
+        <f>I40-K40</f>
         <v>2.2345637107881018</v>
       </c>
       <c r="O40" s="30" t="str">
-        <f t="shared" si="17"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P40" s="5">
-        <f t="shared" si="18"/>
+        <f>N40/M40</f>
         <v>1.7963311108174056</v>
       </c>
       <c r="Q40" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R40" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I40&gt;K40,1-_xlfn.NORM.DIST(I40,K40,M40,1),_xlfn.NORM.DIST(I40,K40,M40,1))</f>
         <v>3.6220936405928716E-2</v>
       </c>
       <c r="S40" s="32" t="str">
-        <f t="shared" si="21"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T40" s="6">
-        <f t="shared" si="22"/>
+        <f>E40/K40</f>
         <v>203.9155999000713</v>
       </c>
       <c r="U40" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f>IF($C40=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T40)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V40" s="4"/>
@@ -6543,7 +6543,7 @@
         <v>40</v>
       </c>
       <c r="F41" s="30">
-        <f t="shared" si="12"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E41)+1)</f>
         <v>32</v>
       </c>
       <c r="G41" s="8">
@@ -6551,7 +6551,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="13"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G41)+1)</f>
         <v>29</v>
       </c>
       <c r="I41" s="8">
@@ -6559,7 +6559,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="14"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I41)+1)</f>
         <v>23</v>
       </c>
       <c r="K41" s="9">
@@ -6567,7 +6567,7 @@
         <v>0.44943930749557348</v>
       </c>
       <c r="L41" s="30">
-        <f t="shared" si="15"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K41)+1)</f>
         <v>27</v>
       </c>
       <c r="M41" s="9">
@@ -6575,35 +6575,35 @@
         <v>0.61791657214945761</v>
       </c>
       <c r="N41" s="9">
-        <f t="shared" si="16"/>
+        <f>I41-K41</f>
         <v>-0.44943930749557348</v>
       </c>
       <c r="O41" s="30">
-        <f t="shared" si="17"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N41)+1)</f>
         <v>22</v>
       </c>
       <c r="P41" s="5">
-        <f t="shared" si="18"/>
+        <f>N41/M41</f>
         <v>-0.72734625959645904</v>
       </c>
       <c r="Q41" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P41)+1)</f>
         <v>26</v>
       </c>
       <c r="R41" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I41&gt;K41,1-_xlfn.NORM.DIST(I41,K41,M41,1),_xlfn.NORM.DIST(I41,K41,M41,1))</f>
         <v>0.23350693326254907</v>
       </c>
       <c r="S41" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R41)+1)</f>
         <v>22</v>
       </c>
       <c r="T41" s="6">
-        <f t="shared" si="22"/>
+        <f>E41/K41</f>
         <v>88.999781133727296</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C41=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T41)+1)</f>
         <v>1</v>
       </c>
       <c r="V41" s="4"/>
@@ -6629,7 +6629,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="30" t="str">
-        <f t="shared" si="12"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G42" s="8">
@@ -6637,7 +6637,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="8" t="str">
-        <f t="shared" si="13"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I42" s="8">
@@ -6645,7 +6645,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="8" t="str">
-        <f t="shared" si="14"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K42" s="9">
@@ -6653,7 +6653,7 @@
         <v>0.23076923076923078</v>
       </c>
       <c r="L42" s="30" t="str">
-        <f t="shared" si="15"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M42" s="9">
@@ -6661,35 +6661,35 @@
         <v>0.42132504423474315</v>
       </c>
       <c r="N42" s="9">
-        <f t="shared" si="16"/>
+        <f>I42-K42</f>
         <v>-0.23076923076923078</v>
       </c>
       <c r="O42" s="30" t="str">
-        <f t="shared" si="17"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P42" s="5">
-        <f t="shared" si="18"/>
+        <f>N42/M42</f>
         <v>-0.54772255750516619</v>
       </c>
       <c r="Q42" s="10" t="str">
-        <f t="shared" si="19"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R42" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I42&gt;K42,1-_xlfn.NORM.DIST(I42,K42,M42,1),_xlfn.NORM.DIST(I42,K42,M42,1))</f>
         <v>0.2919412103851825</v>
       </c>
       <c r="S42" s="32" t="str">
-        <f t="shared" si="21"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T42" s="6">
-        <f t="shared" si="22"/>
+        <f>E42/K42</f>
         <v>0</v>
       </c>
       <c r="U42" s="4" t="str">
-        <f t="shared" si="23"/>
+        <f>IF($C42=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T42)+1)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V42" s="4"/>
@@ -6715,7 +6715,7 @@
         <v>610</v>
       </c>
       <c r="F43" s="30">
-        <f t="shared" si="12"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E43)+1)</f>
         <v>13</v>
       </c>
       <c r="G43" s="8">
@@ -6723,7 +6723,7 @@
         <v>61</v>
       </c>
       <c r="H43" s="10">
-        <f t="shared" si="13"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G43)+1)</f>
         <v>13</v>
       </c>
       <c r="I43" s="8">
@@ -6731,7 +6731,7 @@
         <v>4</v>
       </c>
       <c r="J43" s="10">
-        <f t="shared" si="14"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I43)+1)</f>
         <v>6</v>
       </c>
       <c r="K43" s="9">
@@ -6739,7 +6739,7 @@
         <v>2.5954788994901623</v>
       </c>
       <c r="L43" s="30">
-        <f t="shared" si="15"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K43)+1)</f>
         <v>13</v>
       </c>
       <c r="M43" s="9">
@@ -6747,35 +6747,35 @@
         <v>1.5361196552748302</v>
       </c>
       <c r="N43" s="9">
-        <f t="shared" si="16"/>
+        <f>I43-K43</f>
         <v>1.4045211005098377</v>
       </c>
       <c r="O43" s="30">
-        <f t="shared" si="17"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N43)+1)</f>
         <v>5</v>
       </c>
       <c r="P43" s="5">
-        <f t="shared" si="18"/>
+        <f>N43/M43</f>
         <v>0.91433053127528141</v>
       </c>
       <c r="Q43" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P43)+1)</f>
         <v>4</v>
       </c>
       <c r="R43" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I43&gt;K43,1-_xlfn.NORM.DIST(I43,K43,M43,1),_xlfn.NORM.DIST(I43,K43,M43,1))</f>
         <v>0.18027159619307453</v>
       </c>
       <c r="S43" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R43)+1)</f>
         <v>24</v>
       </c>
       <c r="T43" s="6">
-        <f t="shared" si="22"/>
+        <f>E43/K43</f>
         <v>235.02406439128598</v>
       </c>
       <c r="U43" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C43=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T43)+1)</f>
         <v>19</v>
       </c>
       <c r="V43" s="4"/>
@@ -6801,7 +6801,7 @@
         <v>180</v>
       </c>
       <c r="F44" s="30">
-        <f t="shared" si="12"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E44)+1)</f>
         <v>26</v>
       </c>
       <c r="G44" s="8">
@@ -6809,7 +6809,7 @@
         <v>18</v>
       </c>
       <c r="H44" s="8">
-        <f t="shared" si="13"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G44)+1)</f>
         <v>26</v>
       </c>
       <c r="I44" s="8">
@@ -6817,7 +6817,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="8">
-        <f t="shared" si="14"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I44)+1)</f>
         <v>18</v>
       </c>
       <c r="K44" s="9">
@@ -6825,7 +6825,7 @@
         <v>0.77946480083496894</v>
       </c>
       <c r="L44" s="30">
-        <f t="shared" si="15"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K44)+1)</f>
         <v>25</v>
       </c>
       <c r="M44" s="9">
@@ -6833,35 +6833,35 @@
         <v>0.85313059319831075</v>
       </c>
       <c r="N44" s="9">
-        <f t="shared" si="16"/>
+        <f>I44-K44</f>
         <v>0.22053519916503106</v>
       </c>
       <c r="O44" s="30">
-        <f t="shared" si="17"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N44)+1)</f>
         <v>11</v>
       </c>
       <c r="P44" s="5">
-        <f t="shared" si="18"/>
+        <f>N44/M44</f>
         <v>0.2585011027892743</v>
       </c>
       <c r="Q44" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P44)+1)</f>
         <v>9</v>
       </c>
       <c r="R44" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I44&gt;K44,1-_xlfn.NORM.DIST(I44,K44,M44,1),_xlfn.NORM.DIST(I44,K44,M44,1))</f>
         <v>0.39801009896921591</v>
       </c>
       <c r="S44" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R44)+1)</f>
         <v>6</v>
       </c>
       <c r="T44" s="6">
-        <f t="shared" si="22"/>
+        <f>E44/K44</f>
         <v>230.92768243951818</v>
       </c>
       <c r="U44" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C44=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T44)+1)</f>
         <v>18</v>
       </c>
       <c r="V44" s="4"/>
@@ -6887,23 +6887,23 @@
         <v>300</v>
       </c>
       <c r="F45" s="30">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E45)+1)</f>
+        <v>21</v>
       </c>
       <c r="G45" s="8">
         <f>SUMIF(Sales!B:B,A45,Sales!D:D)</f>
         <v>30</v>
       </c>
       <c r="H45" s="8">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G45)+1)</f>
+        <v>20</v>
       </c>
       <c r="I45" s="8">
         <f>SUMIF(Prizes!B:B,A45,Prizes!D:D)</f>
         <v>1</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="14"/>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I45)+1)</f>
         <v>18</v>
       </c>
       <c r="K45" s="9">
@@ -6911,43 +6911,43 @@
         <v>1.3879411334843073</v>
       </c>
       <c r="L45" s="30">
-        <f t="shared" si="15"/>
-        <v>20</v>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K45)+1)</f>
+        <v>21</v>
       </c>
       <c r="M45" s="9">
         <f>SQRT(SUMIF(Sales!B:B,A45,Sales!G:G))</f>
         <v>1.1316866919830026</v>
       </c>
       <c r="N45" s="9">
-        <f t="shared" si="16"/>
+        <f>I45-K45</f>
         <v>-0.38794113348430725</v>
       </c>
       <c r="O45" s="30">
-        <f t="shared" si="17"/>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N45)+1)</f>
         <v>19</v>
       </c>
       <c r="P45" s="5">
-        <f t="shared" si="18"/>
+        <f>N45/M45</f>
         <v>-0.34279905934436306</v>
       </c>
       <c r="Q45" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P45)+1)</f>
         <v>17</v>
       </c>
       <c r="R45" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I45&gt;K45,1-_xlfn.NORM.DIST(I45,K45,M45,1),_xlfn.NORM.DIST(I45,K45,M45,1))</f>
         <v>0.36587481683043532</v>
       </c>
       <c r="S45" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R45)+1)</f>
         <v>10</v>
       </c>
       <c r="T45" s="6">
-        <f t="shared" si="22"/>
+        <f>E45/K45</f>
         <v>216.14749556912093</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C45=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T45)+1)</f>
         <v>9</v>
       </c>
       <c r="V45" s="4"/>
@@ -6973,7 +6973,7 @@
         <v>350</v>
       </c>
       <c r="F46" s="30">
-        <f t="shared" si="12"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E46)+1)</f>
         <v>17</v>
       </c>
       <c r="G46" s="8">
@@ -6981,7 +6981,7 @@
         <v>35</v>
       </c>
       <c r="H46" s="8">
-        <f t="shared" si="13"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G46)+1)</f>
         <v>17</v>
       </c>
       <c r="I46" s="8">
@@ -6989,7 +6989,7 @@
         <v>2</v>
       </c>
       <c r="J46" s="8">
-        <f t="shared" si="14"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I46)+1)</f>
         <v>11</v>
       </c>
       <c r="K46" s="9">
@@ -6997,7 +6997,7 @@
         <v>1.7130713531328208</v>
       </c>
       <c r="L46" s="30">
-        <f t="shared" si="15"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K46)+1)</f>
         <v>18</v>
       </c>
       <c r="M46" s="9">
@@ -7005,35 +7005,35 @@
         <v>1.2443964039556024</v>
       </c>
       <c r="N46" s="9">
-        <f t="shared" si="16"/>
+        <f>I46-K46</f>
         <v>0.28692864686717923</v>
       </c>
       <c r="O46" s="30">
-        <f t="shared" si="17"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N46)+1)</f>
         <v>9</v>
       </c>
       <c r="P46" s="5">
-        <f t="shared" si="18"/>
+        <f>N46/M46</f>
         <v>0.23057656383055272</v>
       </c>
       <c r="Q46" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P46)+1)</f>
         <v>10</v>
       </c>
       <c r="R46" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I46&gt;K46,1-_xlfn.NORM.DIST(I46,K46,M46,1),_xlfn.NORM.DIST(I46,K46,M46,1))</f>
         <v>0.4088218881933674</v>
       </c>
       <c r="S46" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R46)+1)</f>
         <v>5</v>
       </c>
       <c r="T46" s="6">
-        <f t="shared" si="22"/>
+        <f>E46/K46</f>
         <v>204.31139622989377</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" si="23"/>
+        <f>IF($C46=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T46)+1)</f>
         <v>3</v>
       </c>
       <c r="V46" s="4"/>
@@ -7059,23 +7059,23 @@
         <v>250</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="12"/>
-        <v>22</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E47)+1)</f>
+        <v>23</v>
       </c>
       <c r="G47" s="10">
         <f>SUMIF(Sales!B:B,A47,Sales!D:D)</f>
         <v>25</v>
       </c>
       <c r="H47" s="10">
-        <f t="shared" si="13"/>
-        <v>22</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G47)+1)</f>
+        <v>23</v>
       </c>
       <c r="I47" s="10">
         <f>SUMIF(Prizes!B:B,A47,Prizes!D:D)</f>
         <v>0</v>
       </c>
       <c r="J47" s="10">
-        <f t="shared" si="14"/>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I47)+1)</f>
         <v>23</v>
       </c>
       <c r="K47" s="5">
@@ -7083,43 +7083,43 @@
         <v>1.184672257882758</v>
       </c>
       <c r="L47" s="6">
-        <f t="shared" si="15"/>
-        <v>22</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K47)+1)</f>
+        <v>23</v>
       </c>
       <c r="M47" s="5">
         <f>SQRT(SUMIF(Sales!B:B,A47,Sales!G:G))</f>
         <v>1.0386412070417264</v>
       </c>
       <c r="N47" s="5">
-        <f t="shared" si="16"/>
+        <f>I47-K47</f>
         <v>-1.184672257882758</v>
       </c>
       <c r="O47" s="6">
-        <f t="shared" si="17"/>
-        <v>29</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N47)+1)</f>
+        <v>28</v>
       </c>
       <c r="P47" s="5">
-        <f t="shared" si="18"/>
+        <f>N47/M47</f>
         <v>-1.1405981679245709</v>
       </c>
       <c r="Q47" s="10">
-        <f t="shared" si="19"/>
-        <v>31</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P47)+1)</f>
+        <v>30</v>
       </c>
       <c r="R47" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I47&gt;K47,1-_xlfn.NORM.DIST(I47,K47,M47,1),_xlfn.NORM.DIST(I47,K47,M47,1))</f>
         <v>0.12701859000624371</v>
       </c>
       <c r="S47" s="32">
-        <f t="shared" si="21"/>
-        <v>28</v>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R47)+1)</f>
+        <v>27</v>
       </c>
       <c r="T47" s="6">
-        <f t="shared" si="22"/>
+        <f>E47/K47</f>
         <v>211.02882956573922</v>
       </c>
       <c r="U47" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C47=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T47)+1)</f>
         <v>6</v>
       </c>
       <c r="X47" s="4"/>
@@ -7144,23 +7144,23 @@
         <v>300</v>
       </c>
       <c r="F48" s="6">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E48)+1)</f>
+        <v>21</v>
       </c>
       <c r="G48" s="10">
         <f>SUMIF(Sales!B:B,A48,Sales!D:D)</f>
         <v>30</v>
       </c>
       <c r="H48" s="10">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G48)+1)</f>
+        <v>20</v>
       </c>
       <c r="I48" s="10">
         <f>SUMIF(Prizes!B:B,A48,Prizes!D:D)</f>
         <v>2</v>
       </c>
       <c r="J48" s="10">
-        <f t="shared" si="14"/>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I48)+1)</f>
         <v>11</v>
       </c>
       <c r="K48" s="5">
@@ -7168,43 +7168,43 @@
         <v>1.4022344140591172</v>
       </c>
       <c r="L48" s="6">
-        <f t="shared" si="15"/>
-        <v>19</v>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K48)+1)</f>
+        <v>20</v>
       </c>
       <c r="M48" s="5">
         <f>SQRT(SUMIF(Sales!B:B,A48,Sales!G:G))</f>
         <v>1.1263544351603461</v>
       </c>
       <c r="N48" s="5">
-        <f t="shared" si="16"/>
+        <f>I48-K48</f>
         <v>0.5977655859408828</v>
       </c>
       <c r="O48" s="6">
-        <f t="shared" si="17"/>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N48)+1)</f>
         <v>7</v>
       </c>
       <c r="P48" s="5">
-        <f t="shared" si="18"/>
+        <f>N48/M48</f>
         <v>0.53070824536309114</v>
       </c>
       <c r="Q48" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P48)+1)</f>
         <v>6</v>
       </c>
       <c r="R48" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I48&gt;K48,1-_xlfn.NORM.DIST(I48,K48,M48,1),_xlfn.NORM.DIST(I48,K48,M48,1))</f>
         <v>0.29781048568497837</v>
       </c>
       <c r="S48" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R48)+1)</f>
         <v>15</v>
       </c>
       <c r="T48" s="6">
-        <f t="shared" si="22"/>
+        <f>E48/K48</f>
         <v>213.94425710290136</v>
       </c>
       <c r="U48" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C48=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T48)+1)</f>
         <v>8</v>
       </c>
       <c r="X48" s="4"/>
@@ -7226,70 +7226,70 @@
       </c>
       <c r="E49" s="28">
         <f>SUMIF(Sales!B:B,A49,Sales!E:E)</f>
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="F49" s="31">
-        <f t="shared" si="12"/>
-        <v>22</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E49)+1)</f>
+        <v>17</v>
       </c>
       <c r="G49" s="28">
         <f>SUMIF(Sales!B:B,A49,Sales!D:D)</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H49" s="28">
-        <f t="shared" si="13"/>
-        <v>22</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G49)+1)</f>
+        <v>17</v>
       </c>
       <c r="I49" s="28">
         <f>SUMIF(Prizes!B:B,A49,Prizes!D:D)</f>
         <v>0</v>
       </c>
       <c r="J49" s="28">
-        <f t="shared" si="14"/>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I49)+1)</f>
         <v>23</v>
       </c>
       <c r="K49" s="29">
         <f>SUMIF(Sales!B:B,A49,Sales!F:F)</f>
-        <v>1.1080697245444242</v>
+        <v>1.5492461951326595</v>
       </c>
       <c r="L49" s="31">
-        <f t="shared" si="15"/>
-        <v>23</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K49)+1)</f>
+        <v>19</v>
       </c>
       <c r="M49" s="29">
         <f>SQRT(SUMIF(Sales!B:B,A49,Sales!G:G))</f>
-        <v>1.0008960839395842</v>
+        <v>1.1812669413653081</v>
       </c>
       <c r="N49" s="29">
-        <f t="shared" si="16"/>
-        <v>-1.1080697245444242</v>
+        <f>I49-K49</f>
+        <v>-1.5492461951326595</v>
       </c>
       <c r="O49" s="31">
-        <f t="shared" si="17"/>
-        <v>28</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N49)+1)</f>
+        <v>30</v>
       </c>
       <c r="P49" s="5">
-        <f t="shared" si="18"/>
-        <v>-1.1070776900065373</v>
+        <f>N49/M49</f>
+        <v>-1.3115123609080612</v>
       </c>
       <c r="Q49" s="10">
-        <f t="shared" si="19"/>
-        <v>29</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P49)+1)</f>
+        <v>31</v>
       </c>
       <c r="R49" s="17">
-        <f t="shared" si="20"/>
-        <v>0.1341301701833536</v>
+        <f>IF(I49&gt;K49,1-_xlfn.NORM.DIST(I49,K49,M49,1),_xlfn.NORM.DIST(I49,K49,M49,1))</f>
+        <v>9.4842360181836213E-2</v>
       </c>
       <c r="S49" s="32">
-        <f t="shared" si="21"/>
-        <v>26</v>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R49)+1)</f>
+        <v>30</v>
       </c>
       <c r="T49" s="6">
-        <f t="shared" si="22"/>
-        <v>225.61757122529983</v>
+        <f>E49/K49</f>
+        <v>225.91632053034027</v>
       </c>
       <c r="U49" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C49=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T49)+1)</f>
         <v>15</v>
       </c>
       <c r="X49" s="4"/>
@@ -7314,7 +7314,7 @@
         <v>190</v>
       </c>
       <c r="F50" s="31">
-        <f t="shared" si="12"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E50)+1)</f>
         <v>25</v>
       </c>
       <c r="G50" s="28">
@@ -7322,7 +7322,7 @@
         <v>19</v>
       </c>
       <c r="H50" s="28">
-        <f t="shared" si="13"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G50)+1)</f>
         <v>24</v>
       </c>
       <c r="I50" s="28">
@@ -7330,7 +7330,7 @@
         <v>3</v>
       </c>
       <c r="J50" s="28">
-        <f t="shared" si="14"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I50)+1)</f>
         <v>10</v>
       </c>
       <c r="K50" s="29">
@@ -7338,7 +7338,7 @@
         <v>0.6788730060179704</v>
       </c>
       <c r="L50" s="31">
-        <f t="shared" si="15"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K50)+1)</f>
         <v>26</v>
       </c>
       <c r="M50" s="29">
@@ -7346,35 +7346,35 @@
         <v>0.79230007491312338</v>
       </c>
       <c r="N50" s="29">
-        <f t="shared" si="16"/>
+        <f>I50-K50</f>
         <v>2.3211269939820296</v>
       </c>
       <c r="O50" s="31">
-        <f t="shared" si="17"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N50)+1)</f>
         <v>2</v>
       </c>
       <c r="P50" s="5">
-        <f t="shared" si="18"/>
+        <f>N50/M50</f>
         <v>2.9296059251749331</v>
       </c>
       <c r="Q50" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P50)+1)</f>
         <v>1</v>
       </c>
       <c r="R50" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I50&gt;K50,1-_xlfn.NORM.DIST(I50,K50,M50,1),_xlfn.NORM.DIST(I50,K50,M50,1))</f>
         <v>1.6969605821705036E-3</v>
       </c>
       <c r="S50" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R50)+1)</f>
         <v>33</v>
       </c>
       <c r="T50" s="6">
-        <f t="shared" si="22"/>
+        <f>E50/K50</f>
         <v>279.87561490251761</v>
       </c>
       <c r="U50" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C50=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T50)+1)</f>
         <v>30</v>
       </c>
       <c r="X50" s="4"/>
@@ -7399,7 +7399,7 @@
         <v>10</v>
       </c>
       <c r="F51" s="31">
-        <f t="shared" si="12"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E51)+1)</f>
         <v>33</v>
       </c>
       <c r="G51" s="28">
@@ -7407,7 +7407,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="28">
-        <f t="shared" si="13"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G51)+1)</f>
         <v>33</v>
       </c>
       <c r="I51" s="28">
@@ -7415,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="28">
-        <f t="shared" si="14"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I51)+1)</f>
         <v>23</v>
       </c>
       <c r="K51" s="29">
@@ -7423,7 +7423,7 @@
         <v>4.046242774566474E-2</v>
       </c>
       <c r="L51" s="31">
-        <f t="shared" si="15"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K51)+1)</f>
         <v>33</v>
       </c>
       <c r="M51" s="29">
@@ -7431,35 +7431,35 @@
         <v>0.19704116241687067</v>
       </c>
       <c r="N51" s="29">
-        <f t="shared" si="16"/>
+        <f>I51-K51</f>
         <v>-4.046242774566474E-2</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" si="17"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N51)+1)</f>
         <v>12</v>
       </c>
       <c r="P51" s="5">
-        <f t="shared" si="18"/>
+        <f>N51/M51</f>
         <v>-0.20535012709710013</v>
       </c>
       <c r="Q51" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P51)+1)</f>
         <v>14</v>
       </c>
       <c r="R51" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I51&gt;K51,1-_xlfn.NORM.DIST(I51,K51,M51,1),_xlfn.NORM.DIST(I51,K51,M51,1))</f>
         <v>0.41864929133648948</v>
       </c>
       <c r="S51" s="32">
-        <f t="shared" si="21"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R51)+1)</f>
         <v>3</v>
       </c>
       <c r="T51" s="6">
-        <f t="shared" si="22"/>
+        <f>E51/K51</f>
         <v>247.14285714285714</v>
       </c>
       <c r="U51" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C51=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T51)+1)</f>
         <v>25</v>
       </c>
       <c r="X51" s="4"/>
@@ -7484,7 +7484,7 @@
         <v>100</v>
       </c>
       <c r="F52" s="31">
-        <f t="shared" si="12"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,E:E,"&gt;"&amp;E52)+1)</f>
         <v>28</v>
       </c>
       <c r="G52" s="28">
@@ -7492,7 +7492,7 @@
         <v>10</v>
       </c>
       <c r="H52" s="28">
-        <f t="shared" si="13"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,G:G,"&gt;"&amp;G52)+1)</f>
         <v>28</v>
       </c>
       <c r="I52" s="28">
@@ -7500,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="28">
-        <f t="shared" si="14"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,I:I,"&gt;"&amp;I52)+1)</f>
         <v>23</v>
       </c>
       <c r="K52" s="29">
@@ -7508,7 +7508,7 @@
         <v>0.44117647058823534</v>
       </c>
       <c r="L52" s="31">
-        <f t="shared" si="15"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,K:K,"&gt;"&amp;K52)+1)</f>
         <v>28</v>
       </c>
       <c r="M52" s="29">
@@ -7516,35 +7516,35 @@
         <v>0.6273743825794571</v>
       </c>
       <c r="N52" s="29">
-        <f t="shared" si="16"/>
+        <f>I52-K52</f>
         <v>-0.44117647058823534</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="17"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,N:N,"&gt;"&amp;N52)+1)</f>
         <v>21</v>
       </c>
       <c r="P52" s="29">
-        <f t="shared" si="18"/>
+        <f>N52/M52</f>
         <v>-0.70321084640774323</v>
       </c>
       <c r="Q52" s="10">
-        <f t="shared" si="19"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,P:P,"&gt;"&amp;P52)+1)</f>
         <v>25</v>
       </c>
       <c r="R52" s="17">
-        <f t="shared" si="20"/>
+        <f>IF(I52&gt;K52,1-_xlfn.NORM.DIST(I52,K52,M52,1),_xlfn.NORM.DIST(I52,K52,M52,1))</f>
         <v>0.24096218039643846</v>
       </c>
       <c r="S52" s="77">
-        <f t="shared" si="21"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,R:R,"&gt;"&amp;R52)+1)</f>
         <v>21</v>
       </c>
       <c r="T52" s="6">
-        <f t="shared" si="22"/>
+        <f>E52/K52</f>
         <v>226.66666666666666</v>
       </c>
       <c r="U52" s="10">
-        <f t="shared" si="23"/>
+        <f>IF($C52=0," ",COUNTIFS($C:$C,1,T:T,"&lt;"&amp;T52)+1)</f>
         <v>17</v>
       </c>
     </row>
@@ -7976,8 +7976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8500,7 +8500,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="3">
-        <f>F17/D17</f>
+        <f t="shared" ref="G17:G22" si="3">F17/D17</f>
         <v>5.4545454545454543E-2</v>
       </c>
       <c r="H17" s="27">
@@ -8531,7 +8531,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="3">
-        <f>F18/D18</f>
+        <f t="shared" si="3"/>
         <v>4.046242774566474E-2</v>
       </c>
       <c r="H18" s="27">
@@ -8562,7 +8562,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="3">
-        <f>F19/D19</f>
+        <f t="shared" si="3"/>
         <v>4.4117647058823532E-2</v>
       </c>
       <c r="H19" s="27">
@@ -8593,7 +8593,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="3">
-        <f>F20/D20</f>
+        <f t="shared" si="3"/>
         <v>5.3691275167785234E-2</v>
       </c>
       <c r="H20" s="27">
@@ -8624,7 +8624,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="3">
-        <f>F21/D21</f>
+        <f t="shared" si="3"/>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="H21" s="27">
@@ -8655,7 +8655,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="3">
-        <f>F22/D22</f>
+        <f t="shared" si="3"/>
         <v>2.7932960893854747E-2</v>
       </c>
       <c r="H22" s="27">
@@ -8687,8 +8687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L396"/>
   <sheetViews>
-    <sheetView topLeftCell="A345" workbookViewId="0">
-      <selection activeCell="K376" sqref="K376"/>
+    <sheetView topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="H400" sqref="H400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17400,7 +17400,7 @@
         <v>322</v>
       </c>
       <c r="B323">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C323" s="11">
         <v>18</v>
@@ -21771,7 +21771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>